<commit_message>
add function for finding location words and test dataset
</commit_message>
<xml_diff>
--- a/server/tests/tweets.xlsx
+++ b/server/tests/tweets.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="489">
   <si>
     <t>id</t>
   </si>
@@ -347,19 +347,8 @@
     <t xml:space="preserve">Πυροσβέστες  Αϊ Βασίληδες, της 3ης ΕΜΑΚ και του Σωματείου Πυροσβεστών Ηρακλείου Τρεις Παίδες εν Καμίνω έβαλαν τα γιορτινά τους και ανταποκρίθηκαν άμεσα στο κάλεσμα των παιδιών στον προαύλιο χώρο της ΠαιδοΟγκολογικής Κλινικής του ΠαΓΝΗ Κρήτης. </t>
   </si>
   <si>
-    <t>Απεγκλωβίστηκε μια γυναίκα από ΕΙΧ όχημα, συνεπεία τροχαίου, ύστερα από σύγκρουση με έτερο όχημα, πλησίον του κόμβου Δωρικού επί της Ε.Ο. ΑλεξανδρούποληςΒΙ.ΠΕ Αλεξανδρούπολης, Έβρου.
-Επιχείρησαν 4 πυροσβέστες με 2 οχήματα.</t>
-  </si>
-  <si>
     <t>Ολοκληρώθηκε ο απεγκλωβισμός ενός ατόμου από Ε.Ι.Χ. όχημα  και παραδόθηκε στο ΕΚΑΒ, συνεπεία τροχαίου, ύστερα από σύγκρουση με έτερο ΕΙΧ όχημα, επί της οδού Στρατάρχου Αλεξάνδρου Παπάγου, στον Εύοσμο Θεσσαλονίκης. 
 Επιχείρησαν 5 πυροσβέστες με 2 οχήματα.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12.598 στελέχη υπηρεσιών έλαβαν πιστοποιημένη εκπαίδευση από την Πυροσβεστική Υπηρεσία Διεθνούς Αερολιμένα Αθηνών  Ελευθέριος Βενιζέλος.
-Σχετικό Δελτίο Τύπου θα βρείτε  </t>
-  </si>
-  <si>
-    <t>Ολοκληρώθηκε η επιχείρηση ανεύρεσης άνδρα στην περιοχή Χρυσοκελλαριά, του δήμου Πύλου  Νέστορος, όπου και παρελήφθη από ασθενοφόρο του ΕΚΑΒ για προληπτικούς λόγους.</t>
   </si>
   <si>
     <t>Υπό μερικό έλεγχο τέθηκε η πυρκαγιά σε ισόγειο χώρο κτιρίου, επί της οδού Καλλέργη στην Αθήνα.</t>
@@ -1391,294 +1380,39 @@
     <t>woi</t>
   </si>
   <si>
-    <t>Περδίκκα Πτολεμαΐδας</t>
-  </si>
-  <si>
-    <t>Κρυονέρι Αττικής</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Αποστόλου Παύλου Θεσσαλονίκη</t>
-  </si>
-  <si>
-    <t>Σόλωνος Μενεμένη Θεσσαλονίκης</t>
-  </si>
-  <si>
-    <t>Ιβήρων Αθήνα</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Π.Υ. Ρεθύμνου</t>
-  </si>
-  <si>
-    <t>Μύρων Αθήνα</t>
-  </si>
-  <si>
-    <t>Γούμερο Ηλείας</t>
-  </si>
-  <si>
     <t>νήσου Ερεικούσσας</t>
   </si>
   <si>
-    <t>Καστέλλα Πειραιώς</t>
-  </si>
-  <si>
-    <t>Λιχάδα Ευβοίας</t>
-  </si>
-  <si>
-    <t>Βασιλική Λευκάδας</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> νήσου Ερεικούσας</t>
-  </si>
-  <si>
-    <t>Πάλιουρα  δήμο Διρφύων Μεσσαπίων Ευβοίας</t>
-  </si>
-  <si>
-    <t>Κρήτη</t>
-  </si>
-  <si>
     <t>Κορινθία</t>
   </si>
   <si>
-    <t>Δραπετσώνα</t>
-  </si>
-  <si>
     <t>Αττικής</t>
   </si>
   <si>
-    <t>Κορινθία Ηλεία</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Λευκίμμη Κέρκυρας</t>
-  </si>
-  <si>
-    <t>Φαράγγι της Γκούρας  Φυλή Αττικής</t>
-  </si>
-  <si>
-    <t>Κατερίνης Πιερίας</t>
-  </si>
-  <si>
-    <t>Αιγάλεω</t>
-  </si>
-  <si>
-    <t>Άγιος Στέφανος Αυλιωτών Κέρκυρας</t>
-  </si>
-  <si>
-    <t>Ελευθερίου Βενιζέλου Πειραιά</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Κωστή Παλαμά Δραπετσώνα</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Διεθνή Αερολιμένα Αθηνών </t>
-  </si>
-  <si>
-    <t>Μ. Αλεξάνδρου Θέρμης Θεσσαλονίκης</t>
-  </si>
-  <si>
-    <t>Θηβών και Πέτρου Ράλλη Αιγάλεω Αττικής</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ύδατα Στυγός Καλαβρύτων</t>
-  </si>
-  <si>
-    <t>Χαριλάου Τρικούπη και Ναυαρίνου  Αθηναίων Αττικής</t>
-  </si>
-  <si>
-    <t>Σαμαρίνας  Αχαρνών Αττικής</t>
-  </si>
-  <si>
-    <t>3ης Σεπτεμβρίου Αθήνα</t>
-  </si>
-  <si>
-    <t>Φύλλου Παλαμά Καρδίτσας</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ιαλυσού </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Αγ. Φωτεινής Ν. Σμύρνη Αττικής</t>
-  </si>
-  <si>
-    <t>Ελασιδών Αθήνα</t>
-  </si>
-  <si>
-    <t>Λεωφόρου Μαραθώνος Νέα Μάκρη Αττικής</t>
-  </si>
-  <si>
-    <t>Χερσόνησος Χερσονήσου Κρήτης</t>
-  </si>
-  <si>
-    <t>Καλλέργη Αθήνα</t>
-  </si>
-  <si>
-    <t>Χρυσοκελλαριά Πύλου  Νέστορος</t>
-  </si>
-  <si>
-    <t>Διεθνούς Αερολιμένα Αθηνών  Ελευθέριος Βενιζέλος</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Στρατάρχου Αλεξάνδρου Παπάγου Εύοσμο Θεσσαλονίκης</t>
-  </si>
-  <si>
-    <t>Δωρικού Ε.Ο. ΑλεξανδρούποληςΒΙ.ΠΕ Αλεξανδρούπολης Έβρου.</t>
-  </si>
-  <si>
     <t>ΠαιδοΟγκολογικής Κλινικής ΠαΓΝΗ Κρήτης</t>
   </si>
   <si>
-    <t>Γαλήνης και Ρόδων Εκάλη Αττικής</t>
-  </si>
-  <si>
-    <t>Ε.Ο. Χρυσοπηγής  Λακκωμάτων Φαρρών Αχαΐας</t>
-  </si>
-  <si>
-    <t>Λάρισα</t>
-  </si>
-  <si>
-    <t>Πλατύ Αλεξάνδρειας Ημαθίας</t>
-  </si>
-  <si>
     <t>Δ.Ε. Λιβαδίου Ελασσόνας της Π.Ε. Λάρισας</t>
   </si>
   <si>
-    <t>Ελ. Βενιζέλου Πέραμα Αττικής</t>
-  </si>
-  <si>
-    <t>Συνταγματάρχου Δαβάκη και Σοφοκλέους Καλλιθέα Αττικής</t>
-  </si>
-  <si>
-    <t>Σιάτοστας  Κνίδης Βοΐου Κοζάνης</t>
-  </si>
-  <si>
-    <t>Ασπρόπυργο Αττικής</t>
-  </si>
-  <si>
-    <t>Μονής Πετράκη Αθήνα</t>
-  </si>
-  <si>
-    <t>Κωννου Παλαιολόγου Νέα Ερυθραία Αττικής</t>
-  </si>
-  <si>
-    <t>Αγίου Μελετίου Αθήνα</t>
-  </si>
-  <si>
-    <t>Νικήτα Πειραιά</t>
-  </si>
-  <si>
-    <t>Καθαρό Λασιθίου Κρήτης</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Νάουσα Ημαθίας </t>
-  </si>
-  <si>
-    <t>ΑθηνώνΚορίνθου στην Κακιά Σκάλα Μεγάρων Σήραγγα Ευπαλίνος</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ν. Παπαδημητρίου Καμένα Βούρλα Φθιωτιδας  </t>
-  </si>
-  <si>
-    <t>Πάφου Αμαρουσίου Αττικής</t>
-  </si>
-  <si>
-    <t>Αγρινίου Πεύκης Αττικής</t>
-  </si>
-  <si>
-    <t>Μάραθος Ηράκλειο Κρήτης</t>
-  </si>
-  <si>
-    <t>Αναξάρχου Ξάνθης</t>
-  </si>
-  <si>
-    <t>Λευκάδας Κορωπί</t>
-  </si>
-  <si>
-    <t>Κυπρίων Αγωνιστών Μαρούσι Αττικής</t>
-  </si>
-  <si>
-    <t>Άνδρου Κορωπί</t>
-  </si>
-  <si>
-    <t>Δαύλειας Λιβαδειά Βοιωτίας</t>
-  </si>
-  <si>
-    <t>Σεράφη Αθηναίων</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Θεοδωριανά Άρτας </t>
-  </si>
-  <si>
-    <t>Λ. Συγγρού Αθήνα</t>
-  </si>
-  <si>
-    <t>Εσπερίδων Κηφισιά</t>
-  </si>
-  <si>
-    <t>17ης Οκτωβρίου Νάουσα Ημαθίας</t>
-  </si>
-  <si>
-    <t>Λεωφόρου Δημοκρατίας Κερατσίνι Αττικής</t>
-  </si>
-  <si>
-    <t>Κουτσουρά Ιεράπετρας</t>
-  </si>
-  <si>
-    <t>Μαράσια Έβρου</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Πεταλούδων Ρόδου </t>
-  </si>
-  <si>
     <t>Λαμία</t>
   </si>
   <si>
     <t>Αγρίνιο</t>
   </si>
   <si>
-    <t xml:space="preserve">Ηράκλειο </t>
-  </si>
-  <si>
     <t>Μυτιλήνη</t>
   </si>
   <si>
-    <t xml:space="preserve">Καβάλας Ξάνθης </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ημαθίας </t>
-  </si>
-  <si>
     <t>Γράμμου Καστοριάς</t>
   </si>
   <si>
-    <t xml:space="preserve">Περιφέρεια Πελοποννήσου </t>
-  </si>
-  <si>
     <t>Αρκαδίας Κορινθίας</t>
   </si>
   <si>
-    <t xml:space="preserve">Πέραμα Αττικής </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Λιοσίων </t>
-  </si>
-  <si>
     <t>Γεράνια Όρη</t>
   </si>
   <si>
-    <t xml:space="preserve">Θρακομακεδόνες </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Θεσσαλονίκης </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Λ. Αθηνών </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Πετρούπολη </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Λ. Μεσογείων </t>
-  </si>
-  <si>
     <t>Καμίνια</t>
   </si>
   <si>
@@ -1691,27 +1425,12 @@
     <t>Ν. Φιλαδέλφεια</t>
   </si>
   <si>
-    <t xml:space="preserve">Αιτωλικού </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Φθιώτιδας </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Δεκελείας Κηφισιά </t>
-  </si>
-  <si>
     <t>Λ. Μαρκοπούλου</t>
   </si>
   <si>
     <t>Δήμου Αθηναίων</t>
   </si>
   <si>
-    <t xml:space="preserve">Αθήνας </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Πάτρα </t>
-  </si>
-  <si>
     <t>Λ. Κατεχάκη</t>
   </si>
   <si>
@@ -1724,18 +1443,9 @@
     <t>Κύμη Ευβοίας</t>
   </si>
   <si>
-    <t xml:space="preserve">Ηλεία </t>
-  </si>
-  <si>
     <t>Μεσσηνία</t>
   </si>
   <si>
-    <t xml:space="preserve">Αρτέμιδα </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Γλυφάδας </t>
-  </si>
-  <si>
     <t>Λέσβο</t>
   </si>
   <si>
@@ -1751,9 +1461,6 @@
     <t>Μαγνησίας</t>
   </si>
   <si>
-    <t xml:space="preserve">Πρέβεζας </t>
-  </si>
-  <si>
     <t>Στερεάς Ελλάδας</t>
   </si>
   <si>
@@ -1761,6 +1468,305 @@
   </si>
   <si>
     <t>Κέρκυρα</t>
+  </si>
+  <si>
+    <t>λίμνη Περδίκκα Πτολεμαΐδας</t>
+  </si>
+  <si>
+    <t>στο Κρυονέρι Αττικής</t>
+  </si>
+  <si>
+    <t>επί της Αποστόλου Παύλου στη Θεσσαλονίκη</t>
+  </si>
+  <si>
+    <t>επί της οδού Σόλωνος στη Μενεμένη Θεσσαλονίκης</t>
+  </si>
+  <si>
+    <t>επί της οδού Ιβήρων στην Αθήνα</t>
+  </si>
+  <si>
+    <t>Π.Υ. Ρεθύμνου</t>
+  </si>
+  <si>
+    <t>επί της οδού Μύρων στην Αθήνα</t>
+  </si>
+  <si>
+    <t>στην περιοχή Γούμερο νομού Ηλείας</t>
+  </si>
+  <si>
+    <t>κοινότητα Πάλιουρα στο δήμο Διρφύων Μεσσαπίων Ευβοίας</t>
+  </si>
+  <si>
+    <t>στην Κρήτη</t>
+  </si>
+  <si>
+    <t>Φαράγγι της Γκούρας στη Φυλή Αττικής</t>
+  </si>
+  <si>
+    <t>στην Δραπετσώνα</t>
+  </si>
+  <si>
+    <t>στην Καστέλλα Πειραιώς</t>
+  </si>
+  <si>
+    <t>επί της οδού Ελευθερίου Βενιζέλου στον Πειραιά</t>
+  </si>
+  <si>
+    <t>στη Δραπετσώνα</t>
+  </si>
+  <si>
+    <t>στο Διεθνή Αερολιμένα Αθηνών</t>
+  </si>
+  <si>
+    <t>επί της οδού Μ. Αλεξάνδρου στο δήμο Θέρμης Θεσσαλονίκης</t>
+  </si>
+  <si>
+    <t>στο δήμο Κατερίνης Πιερίας</t>
+  </si>
+  <si>
+    <t>στο Αιγάλεω</t>
+  </si>
+  <si>
+    <t>επί των οδών Θηβών και Πέτρου Ράλλη στο Αιγάλεω Αττικής</t>
+  </si>
+  <si>
+    <t>στην περιοχή Άγιος Στέφανος Αυλιωτών Κέρκυρας</t>
+  </si>
+  <si>
+    <t>των οδών Χαριλάου Τρικούπη και Ναυαρίνου στο δήμο Αθηναίων Αττικής</t>
+  </si>
+  <si>
+    <t>επί της οδού Σαμαρίνας στο δήμο Αχαρνών Αττικής</t>
+  </si>
+  <si>
+    <t>στην περιοχή Λιχάδα Ευβοίας</t>
+  </si>
+  <si>
+    <t>δημοτική κοινότητα Φύλλου του δήμου Παλαμά Καρδίτσας</t>
+  </si>
+  <si>
+    <t>δημοτική κοινότητα Ιαλυσού της Ρόδου</t>
+  </si>
+  <si>
+    <t>στην περιοχή Μαράσια Έβρου</t>
+  </si>
+  <si>
+    <t>δασάκι Κουτσουρά του δήμου Ιεράπετρας</t>
+  </si>
+  <si>
+    <t>επί της Λεωφόρου Δημοκρατίας στο Κερατσίνι Αττικής</t>
+  </si>
+  <si>
+    <t>επί της οδού 17ης Οκτωβρίου στη Νάουσα Ημαθίας</t>
+  </si>
+  <si>
+    <t>στο Υπουργείο Κλιματικής Κρίσης</t>
+  </si>
+  <si>
+    <t>επί της οδού Εσπερίδων στη Κηφισιά</t>
+  </si>
+  <si>
+    <t>στην Αττική</t>
+  </si>
+  <si>
+    <t>στην περιοχή Βασιλική Λευκάδας</t>
+  </si>
+  <si>
+    <t>επί της Λ. Συγγρού στην Αθήνα</t>
+  </si>
+  <si>
+    <t>επί της οδού Σεράφη στο Αθηναίων</t>
+  </si>
+  <si>
+    <t>στην περιοχή Δαύλειας στη Λιβαδειά Βοιωτίας</t>
+  </si>
+  <si>
+    <t>επί της οδού Άνδρου στο Κορωπί</t>
+  </si>
+  <si>
+    <t>στο Μαρούσι στο Διακοπτό Αχαΐας</t>
+  </si>
+  <si>
+    <t>επί της οδού Κυπρίων Αγωνιστών στο Μαρούσι Αττικής</t>
+  </si>
+  <si>
+    <t>επί της οδού Λευκάδας στο Κορωπί</t>
+  </si>
+  <si>
+    <t>επί της οδού Αναξάρχου στο δήμο της Ξάνθης</t>
+  </si>
+  <si>
+    <t>στη Νέα Ποτίδαια Χαλκιδικής</t>
+  </si>
+  <si>
+    <t>στην περιοχή Μάραθος στο Ηράκλειο Κρήτης</t>
+  </si>
+  <si>
+    <t>επί της οδού Αγρινίου στο δήμο Πεύκης Αττικής</t>
+  </si>
+  <si>
+    <t>επί της οδού Πάφου στο δήμο Αμαρουσίου Αττικής</t>
+  </si>
+  <si>
+    <t>στην Ε.Ο. ΑθηνώνΚορίνθου στην Κακιά Σκάλα Μεγάρων Σήραγγα Ευπαλίνος</t>
+  </si>
+  <si>
+    <t>στην περιοχή Καθαρό Λασιθίου</t>
+  </si>
+  <si>
+    <t>επί της οδού Αγίου Μελετίου στην Αθήνα</t>
+  </si>
+  <si>
+    <t>επί της οδού Νικήτα στον Πειραιά</t>
+  </si>
+  <si>
+    <t>επί της οδού Κωννου Παλαιολόγου στη Νέα Ερυθραία Αττικής</t>
+  </si>
+  <si>
+    <t>επί της οδού Μονής Πετράκη στην Αθήνα</t>
+  </si>
+  <si>
+    <t>στον Ασπρόπυργο Αττικής</t>
+  </si>
+  <si>
+    <t>στη συμβολή των οδών Συνταγματάρχου Δαβάκη και Σοφοκλέους στην Καλλιθέα Αττικής</t>
+  </si>
+  <si>
+    <t>επί της οδού Ελ. Βενιζέλου στο Πέραμα Αττικής</t>
+  </si>
+  <si>
+    <t>στην περιοχή Πλατύ δήμου Αλεξάνδρειας Ημαθίας</t>
+  </si>
+  <si>
+    <t>στη Λάρισα</t>
+  </si>
+  <si>
+    <t>στη συμβολή των οδών Γαλήνης και Ρόδων στην Εκάλη Αττικής</t>
+  </si>
+  <si>
+    <t>Απεγκλωβίστηκε μια γυναίκα από ΕΙΧ όχημα, συνεπεία τροχαίου, ύστερα από σύγκρουση με έτερο όχημα, πλησίον του κόμβου Δωρικού επί της Ε.Ο. Αλεξανδρούπολης ΒΙ.ΠΕ Αλεξανδρούπολης, Έβρου.
+Επιχείρησαν 4 πυροσβέστες με 2 οχήματα.</t>
+  </si>
+  <si>
+    <t>κόμβου Δωρικού επί της Ε.Ο. Αλεξανδρούπολης ΒΙ.ΠΕ Αλεξανδρούπολης Έβρου</t>
+  </si>
+  <si>
+    <t>επί της οδού Στρατάρχου Αλεξάνδρου Παπάγου στον Εύοσμο Θεσσαλονίκης</t>
+  </si>
+  <si>
+    <t>την Πυροσβεστική Υπηρεσία Διεθνούς Αερολιμένα Αθηνών Ελευθέριος Βενιζέλος</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.598 στελέχη υπηρεσιών έλαβαν πιστοποιημένη εκπαίδευση από την Πυροσβεστική Υπηρεσία Διεθνούς Αερολιμένα Αθηνών Ελευθέριος Βενιζέλος.
+Σχετικό Δελτίο Τύπου θα βρείτε  </t>
+  </si>
+  <si>
+    <t>Ολοκληρώθηκε η επιχείρηση ανεύρεσης άνδρα στην περιοχή Χρυσοκελλαριά, του δήμου Πύλου Νέστορος, όπου και παρελήφθη από ασθενοφόρο του ΕΚΑΒ για προληπτικούς λόγους.</t>
+  </si>
+  <si>
+    <t>στην περιοχή Χρυσοκελλαριά του δήμου Πύλου Νέστορος</t>
+  </si>
+  <si>
+    <t>επί της οδού Καλλέργη στην Αθήνα</t>
+  </si>
+  <si>
+    <t>στην περιοχή επάνω Χερσόνησος του δήμου Χερσονήσου Κρήτης</t>
+  </si>
+  <si>
+    <t>επί της Λεωφόρου Μαραθώνος στη Νέα Μάκρη Αττικής</t>
+  </si>
+  <si>
+    <t>επί της οδού Ελασιδών στην Αθήνα</t>
+  </si>
+  <si>
+    <t>επί της οδού Αγ. Φωτεινής στη Ν. Σμύρνη Αττικής</t>
+  </si>
+  <si>
+    <t>νήσου Ερεικούσας</t>
+  </si>
+  <si>
+    <t>επί της οδού Κωστή Παλαμά στη Δραπετσώνα</t>
+  </si>
+  <si>
+    <t>στη Λευκίμμη Κέρκυρας</t>
+  </si>
+  <si>
+    <t>επί της οδού 3ης Σεπτεμβρίου στην Αθήνα</t>
+  </si>
+  <si>
+    <t>στην περιοχή Ύδατα Στυγός</t>
+  </si>
+  <si>
+    <t>στη Νάουσα Ημαθίας</t>
+  </si>
+  <si>
+    <t>δημοτική κοινότητα Πεταλούδων της Ρόδου</t>
+  </si>
+  <si>
+    <t>στην ορεινή περιοχή Θεοδωριανά Άρτας</t>
+  </si>
+  <si>
+    <t>επί της Επ. οδού Σιάτοστας Κνίδης στο Δήμο Βοΐου Κοζάνης</t>
+  </si>
+  <si>
+    <t>Ε.Ο. Χρυσοπηγής Λακκωμάτων Φαρρών Αχαΐας</t>
+  </si>
+  <si>
+    <t>επί της οδού Ν. Παπαδημητρίου στα Καμένα Βούρλα Φθιωτιδας</t>
+  </si>
+  <si>
+    <t>Καβάλας Ξάνθης</t>
+  </si>
+  <si>
+    <t>Ημαθίας</t>
+  </si>
+  <si>
+    <t>Περιφέρεια Πελοποννήσου</t>
+  </si>
+  <si>
+    <t>Πέραμα Αττικής</t>
+  </si>
+  <si>
+    <t>Λιοσίων</t>
+  </si>
+  <si>
+    <t>Θρακομακεδόνες</t>
+  </si>
+  <si>
+    <t>Θεσσαλονίκης</t>
+  </si>
+  <si>
+    <t>Λ. Αθηνών</t>
+  </si>
+  <si>
+    <t>Πετρούπολη</t>
+  </si>
+  <si>
+    <t>Λ. Μεσογείων</t>
+  </si>
+  <si>
+    <t>Δεκελείας Κηφισιά</t>
+  </si>
+  <si>
+    <t>Αθήνας</t>
+  </si>
+  <si>
+    <t>Πάτρα</t>
+  </si>
+  <si>
+    <t>Ηλεία</t>
+  </si>
+  <si>
+    <t>Αρτέμιδα</t>
+  </si>
+  <si>
+    <t>Γλυφάδας</t>
+  </si>
+  <si>
+    <t>Πρέβεζας</t>
+  </si>
+  <si>
+    <t>Φθιώτιδας</t>
   </si>
 </sst>
 </file>
@@ -2476,27 +2482,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.5703125" customWidth="1"/>
     <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -2527,7 +2533,7 @@
         <v>1.496479736087958E+18</v>
       </c>
       <c r="C3" t="s">
-        <v>363</v>
+        <v>390</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -2544,7 +2550,7 @@
         <v>1.496462660124226E+18</v>
       </c>
       <c r="C4" t="s">
-        <v>364</v>
+        <v>391</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>5</v>
@@ -2561,7 +2567,7 @@
         <v>1.496205536869728E+18</v>
       </c>
       <c r="C5" t="s">
-        <v>365</v>
+        <v>392</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -2578,7 +2584,7 @@
         <v>1.495619130669556E+18</v>
       </c>
       <c r="C6" t="s">
-        <v>366</v>
+        <v>393</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -2595,7 +2601,7 @@
         <v>1.4955983911113971E+18</v>
       </c>
       <c r="C7" t="s">
-        <v>367</v>
+        <v>394</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -2612,7 +2618,7 @@
         <v>1.4954265751727639E+18</v>
       </c>
       <c r="C8" t="s">
-        <v>368</v>
+        <v>395</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -2629,7 +2635,7 @@
         <v>1.493064014221431E+18</v>
       </c>
       <c r="C9" t="s">
-        <v>369</v>
+        <v>396</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -2646,7 +2652,7 @@
         <v>1.4947228273118001E+18</v>
       </c>
       <c r="C10" t="s">
-        <v>370</v>
+        <v>397</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -2663,7 +2669,7 @@
         <v>1.4946563831443661E+18</v>
       </c>
       <c r="C11" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -2680,7 +2686,7 @@
         <v>1.494552860612256E+18</v>
       </c>
       <c r="C12" t="s">
-        <v>375</v>
+        <v>460</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -2697,7 +2703,7 @@
         <v>1.49431213538766E+18</v>
       </c>
       <c r="C13" t="s">
-        <v>376</v>
+        <v>398</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -2714,7 +2720,7 @@
         <v>1.494038005891445E+18</v>
       </c>
       <c r="C14" t="s">
-        <v>377</v>
+        <v>399</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -2744,9 +2750,6 @@
       <c r="B16">
         <v>1.4933134163999329E+18</v>
       </c>
-      <c r="C16" t="s">
-        <v>381</v>
-      </c>
       <c r="D16" s="6" t="s">
         <v>17</v>
       </c>
@@ -2776,7 +2779,7 @@
         <v>1.4927544793678269E+18</v>
       </c>
       <c r="C18" t="s">
-        <v>382</v>
+        <v>462</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>19</v>
@@ -2793,7 +2796,7 @@
         <v>1.4926786114758661E+18</v>
       </c>
       <c r="C19" t="s">
-        <v>383</v>
+        <v>400</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
@@ -2810,7 +2813,7 @@
         <v>1.4921848652190021E+18</v>
       </c>
       <c r="C20" t="s">
-        <v>379</v>
+        <v>401</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -2827,7 +2830,7 @@
         <v>1.492132092154626E+18</v>
       </c>
       <c r="C21" t="s">
-        <v>372</v>
+        <v>402</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -2844,7 +2847,7 @@
         <v>1.492113436976767E+18</v>
       </c>
       <c r="C22" t="s">
-        <v>387</v>
+        <v>403</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
@@ -2861,7 +2864,7 @@
         <v>1.4920709015417411E+18</v>
       </c>
       <c r="C23" t="s">
-        <v>379</v>
+        <v>404</v>
       </c>
       <c r="D23" t="s">
         <v>24</v>
@@ -2878,7 +2881,7 @@
         <v>1.4920578290704881E+18</v>
       </c>
       <c r="C24" t="s">
-        <v>388</v>
+        <v>461</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>25</v>
@@ -2895,7 +2898,7 @@
         <v>1.491436312951669E+18</v>
       </c>
       <c r="C25" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="D25" t="s">
         <v>26</v>
@@ -2912,7 +2915,7 @@
         <v>1.4911970611692989E+18</v>
       </c>
       <c r="C26" t="s">
-        <v>390</v>
+        <v>406</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>27</v>
@@ -2929,7 +2932,7 @@
         <v>1.4910949816791199E+18</v>
       </c>
       <c r="C27" t="s">
-        <v>384</v>
+        <v>407</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>28</v>
@@ -2946,7 +2949,7 @@
         <v>1.491016054327636E+18</v>
       </c>
       <c r="C28" t="s">
-        <v>385</v>
+        <v>408</v>
       </c>
       <c r="D28" t="s">
         <v>29</v>
@@ -2963,7 +2966,7 @@
         <v>1.4910125643563169E+18</v>
       </c>
       <c r="C29" t="s">
-        <v>391</v>
+        <v>409</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>30</v>
@@ -2980,7 +2983,7 @@
         <v>1.4904666193987011E+18</v>
       </c>
       <c r="C30" t="s">
-        <v>392</v>
+        <v>464</v>
       </c>
       <c r="D30" t="s">
         <v>31</v>
@@ -2997,7 +3000,7 @@
         <v>1.4903946393917281E+18</v>
       </c>
       <c r="C31" t="s">
-        <v>386</v>
+        <v>410</v>
       </c>
       <c r="D31" t="s">
         <v>32</v>
@@ -3014,7 +3017,7 @@
         <v>1.490325110905098E+18</v>
       </c>
       <c r="C32" t="s">
-        <v>392</v>
+        <v>464</v>
       </c>
       <c r="D32" t="s">
         <v>33</v>
@@ -3031,7 +3034,7 @@
         <v>1.490322862565122E+18</v>
       </c>
       <c r="C33" t="s">
-        <v>392</v>
+        <v>464</v>
       </c>
       <c r="D33" t="s">
         <v>34</v>
@@ -3048,7 +3051,7 @@
         <v>1.49013549454977E+18</v>
       </c>
       <c r="C34" t="s">
-        <v>393</v>
+        <v>411</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>35</v>
@@ -3065,7 +3068,7 @@
         <v>1.490121458588213E+18</v>
       </c>
       <c r="C35" t="s">
-        <v>394</v>
+        <v>412</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>36</v>
@@ -3082,7 +3085,7 @@
         <v>1.4899548776105411E+18</v>
       </c>
       <c r="C36" t="s">
-        <v>373</v>
+        <v>413</v>
       </c>
       <c r="D36" t="s">
         <v>37</v>
@@ -3099,7 +3102,7 @@
         <v>1.433366270540386E+18</v>
       </c>
       <c r="C37" t="s">
-        <v>395</v>
+        <v>463</v>
       </c>
       <c r="D37" t="s">
         <v>38</v>
@@ -3116,7 +3119,7 @@
         <v>1.489008039596278E+18</v>
       </c>
       <c r="C38" t="s">
-        <v>396</v>
+        <v>414</v>
       </c>
       <c r="D38" t="s">
         <v>39</v>
@@ -3133,7 +3136,7 @@
         <v>1.4890004792124129E+18</v>
       </c>
       <c r="C39" t="s">
-        <v>397</v>
+        <v>415</v>
       </c>
       <c r="D39" t="s">
         <v>40</v>
@@ -3150,7 +3153,7 @@
         <v>1.4889945235061719E+18</v>
       </c>
       <c r="C40" t="s">
-        <v>441</v>
+        <v>466</v>
       </c>
       <c r="D40" t="s">
         <v>41</v>
@@ -3167,7 +3170,7 @@
         <v>1.4884793944862679E+18</v>
       </c>
       <c r="C41" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
       <c r="D41" t="s">
         <v>42</v>
@@ -3184,7 +3187,7 @@
         <v>1.487915151424725E+18</v>
       </c>
       <c r="C42" t="s">
-        <v>439</v>
+        <v>417</v>
       </c>
       <c r="D42" t="s">
         <v>43</v>
@@ -3201,7 +3204,7 @@
         <v>1.4879134019973079E+18</v>
       </c>
       <c r="C43" t="s">
-        <v>438</v>
+        <v>418</v>
       </c>
       <c r="D43" t="s">
         <v>44</v>
@@ -3218,7 +3221,7 @@
         <v>1.4876847100169869E+18</v>
       </c>
       <c r="C44" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="D44" t="s">
         <v>45</v>
@@ -3234,6 +3237,9 @@
       <c r="B45">
         <v>1.4874136059182001E+18</v>
       </c>
+      <c r="C45" t="s">
+        <v>420</v>
+      </c>
       <c r="D45" t="s">
         <v>46</v>
       </c>
@@ -3249,7 +3255,7 @@
         <v>1.4869962274598871E+18</v>
       </c>
       <c r="C46" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="D46" t="s">
         <v>47</v>
@@ -3279,6 +3285,9 @@
       <c r="B48">
         <v>1.4865907942365839E+18</v>
       </c>
+      <c r="C48" t="s">
+        <v>422</v>
+      </c>
       <c r="D48" t="s">
         <v>49</v>
       </c>
@@ -3294,7 +3303,7 @@
         <v>1.486362281797632E+18</v>
       </c>
       <c r="C49" t="s">
-        <v>434</v>
+        <v>467</v>
       </c>
       <c r="D49" t="s">
         <v>50</v>
@@ -3311,7 +3320,7 @@
         <v>1.486302382766047E+18</v>
       </c>
       <c r="C50" t="s">
-        <v>374</v>
+        <v>423</v>
       </c>
       <c r="D50" t="s">
         <v>51</v>
@@ -3328,7 +3337,7 @@
         <v>1.4862169617344589E+18</v>
       </c>
       <c r="C51" t="s">
-        <v>435</v>
+        <v>424</v>
       </c>
       <c r="D51" t="s">
         <v>52</v>
@@ -3345,7 +3354,7 @@
         <v>1.486125885501673E+18</v>
       </c>
       <c r="C52" t="s">
-        <v>434</v>
+        <v>467</v>
       </c>
       <c r="D52" t="s">
         <v>53</v>
@@ -3362,7 +3371,7 @@
         <v>1.47200486262385E+18</v>
       </c>
       <c r="C53" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="D53" t="s">
         <v>54</v>
@@ -3378,6 +3387,9 @@
       <c r="B54">
         <v>1.4858464273393091E+18</v>
       </c>
+      <c r="C54" t="s">
+        <v>422</v>
+      </c>
       <c r="D54" t="s">
         <v>55</v>
       </c>
@@ -3407,7 +3419,7 @@
         <v>1.4857203264284101E+18</v>
       </c>
       <c r="C56" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="D56" t="s">
         <v>57</v>
@@ -3424,7 +3436,7 @@
         <v>1.4855368766185229E+18</v>
       </c>
       <c r="C57" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="D57" t="s">
         <v>58</v>
@@ -3447,14 +3459,17 @@
         <v>44812.386655092603</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59">
         <v>1.484506180097655E+18</v>
       </c>
-      <c r="D59" t="s">
+      <c r="C59" t="s">
+        <v>428</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E59" s="2">
@@ -3469,7 +3484,7 @@
         <v>1.484430676657164E+18</v>
       </c>
       <c r="C60" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D60" t="s">
         <v>61</v>
@@ -3486,7 +3501,7 @@
         <v>1.4835632394222799E+18</v>
       </c>
       <c r="C61" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D61" t="s">
         <v>62</v>
@@ -3503,7 +3518,7 @@
         <v>1.4834345118536699E+18</v>
       </c>
       <c r="C62" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="D62" t="s">
         <v>63</v>
@@ -3533,6 +3548,9 @@
       <c r="B64">
         <v>1.483088644411998E+18</v>
       </c>
+      <c r="C64" t="s">
+        <v>432</v>
+      </c>
       <c r="D64" t="s">
         <v>65</v>
       </c>
@@ -3548,7 +3566,7 @@
         <v>1.482814735238242E+18</v>
       </c>
       <c r="C65" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="D65" t="s">
         <v>66</v>
@@ -3565,7 +3583,7 @@
         <v>1.4825248905698801E+18</v>
       </c>
       <c r="C66" t="s">
-        <v>426</v>
+        <v>434</v>
       </c>
       <c r="D66" t="s">
         <v>67</v>
@@ -3582,7 +3600,7 @@
         <v>1.4825234506484979E+18</v>
       </c>
       <c r="C67" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
       <c r="D67" t="s">
         <v>68</v>
@@ -3599,7 +3617,7 @@
         <v>1.4825125147055099E+18</v>
       </c>
       <c r="C68" t="s">
-        <v>424</v>
+        <v>470</v>
       </c>
       <c r="D68" t="s">
         <v>69</v>
@@ -3616,7 +3634,7 @@
         <v>1.482454181701108E+18</v>
       </c>
       <c r="C69" t="s">
-        <v>423</v>
+        <v>436</v>
       </c>
       <c r="D69" t="s">
         <v>70</v>
@@ -3633,7 +3651,7 @@
         <v>1.482425824649396E+18</v>
       </c>
       <c r="C70" t="s">
-        <v>422</v>
+        <v>465</v>
       </c>
       <c r="D70" t="s">
         <v>71</v>
@@ -3650,7 +3668,7 @@
         <v>1.4819311112950661E+18</v>
       </c>
       <c r="C71" t="s">
-        <v>421</v>
+        <v>437</v>
       </c>
       <c r="D71" t="s">
         <v>72</v>
@@ -3667,7 +3685,7 @@
         <v>1.481865846884651E+18</v>
       </c>
       <c r="C72" t="s">
-        <v>419</v>
+        <v>438</v>
       </c>
       <c r="D72" t="s">
         <v>73</v>
@@ -3684,7 +3702,7 @@
         <v>1.448482938979594E+18</v>
       </c>
       <c r="C73" t="s">
-        <v>420</v>
+        <v>439</v>
       </c>
       <c r="D73" t="s">
         <v>74</v>
@@ -3701,7 +3719,7 @@
         <v>1.481845556083372E+18</v>
       </c>
       <c r="C74" t="s">
-        <v>419</v>
+        <v>438</v>
       </c>
       <c r="D74" t="s">
         <v>75</v>
@@ -3718,7 +3736,7 @@
         <v>1.4814368369165151E+18</v>
       </c>
       <c r="C75" t="s">
-        <v>418</v>
+        <v>440</v>
       </c>
       <c r="D75" t="s">
         <v>76</v>
@@ -3735,7 +3753,7 @@
         <v>1.4814352425734799E+18</v>
       </c>
       <c r="C76" t="s">
-        <v>417</v>
+        <v>441</v>
       </c>
       <c r="D76" t="s">
         <v>77</v>
@@ -3752,7 +3770,7 @@
         <v>1.4813921562585779E+18</v>
       </c>
       <c r="C77" t="s">
-        <v>416</v>
+        <v>442</v>
       </c>
       <c r="D77" t="s">
         <v>78</v>
@@ -3769,7 +3787,7 @@
         <v>1.4813882358174641E+18</v>
       </c>
       <c r="C78" t="s">
-        <v>415</v>
+        <v>468</v>
       </c>
       <c r="D78" t="s">
         <v>79</v>
@@ -3786,7 +3804,7 @@
         <v>1.480362152947028E+18</v>
       </c>
       <c r="C79" t="s">
-        <v>414</v>
+        <v>443</v>
       </c>
       <c r="D79" t="s">
         <v>80</v>
@@ -3803,7 +3821,7 @@
         <v>1.4803204688130619E+18</v>
       </c>
       <c r="C80" t="s">
-        <v>413</v>
+        <v>444</v>
       </c>
       <c r="D80" t="s">
         <v>81</v>
@@ -3820,7 +3838,7 @@
         <v>1.480310495781474E+18</v>
       </c>
       <c r="C81" t="s">
-        <v>413</v>
+        <v>444</v>
       </c>
       <c r="D81" t="s">
         <v>82</v>
@@ -3837,7 +3855,7 @@
         <v>1.4801211623740291E+18</v>
       </c>
       <c r="C82" t="s">
-        <v>412</v>
+        <v>364</v>
       </c>
       <c r="D82" t="s">
         <v>83</v>
@@ -3854,7 +3872,7 @@
         <v>1.479258790407115E+18</v>
       </c>
       <c r="C83" t="s">
-        <v>411</v>
+        <v>445</v>
       </c>
       <c r="D83" t="s">
         <v>84</v>
@@ -3871,7 +3889,7 @@
         <v>1.479118702964396E+18</v>
       </c>
       <c r="C84" t="s">
-        <v>410</v>
+        <v>446</v>
       </c>
       <c r="D84" t="s">
         <v>85</v>
@@ -3888,7 +3906,7 @@
         <v>1.479035678797279E+18</v>
       </c>
       <c r="C85" t="s">
-        <v>409</v>
+        <v>469</v>
       </c>
       <c r="D85" t="s">
         <v>86</v>
@@ -3933,7 +3951,7 @@
         <v>1.47708230602845E+18</v>
       </c>
       <c r="C88" t="s">
-        <v>408</v>
+        <v>447</v>
       </c>
       <c r="D88" t="s">
         <v>89</v>
@@ -3992,7 +4010,7 @@
         <v>1.476950490072162E+18</v>
       </c>
       <c r="C92" t="s">
-        <v>407</v>
+        <v>363</v>
       </c>
       <c r="D92" t="s">
         <v>93</v>
@@ -4009,10 +4027,10 @@
         <v>1.4769410577409679E+18</v>
       </c>
       <c r="C93" t="s">
-        <v>406</v>
+        <v>449</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>94</v>
+        <v>448</v>
       </c>
       <c r="E93" s="2">
         <v>44561.735682870371</v>
@@ -4026,10 +4044,10 @@
         <v>1.4769342083586911E+18</v>
       </c>
       <c r="C94" t="s">
-        <v>405</v>
+        <v>450</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E94" s="2">
         <v>44561.716782407413</v>
@@ -4043,10 +4061,10 @@
         <v>1.4758449438853161E+18</v>
       </c>
       <c r="C95" t="s">
-        <v>404</v>
+        <v>451</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>96</v>
+        <v>452</v>
       </c>
       <c r="E95" s="2">
         <v>44558.7109837963</v>
@@ -4060,10 +4078,10 @@
         <v>1.475129417219424E+18</v>
       </c>
       <c r="C96" t="s">
-        <v>403</v>
+        <v>454</v>
       </c>
       <c r="D96" t="s">
-        <v>97</v>
+        <v>453</v>
       </c>
       <c r="E96" s="2">
         <v>44556.736504629633</v>
@@ -4077,10 +4095,10 @@
         <v>1.4750229633008351E+18</v>
       </c>
       <c r="C97" t="s">
-        <v>402</v>
+        <v>455</v>
       </c>
       <c r="D97" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E97" s="2">
         <v>44556.442743055559</v>
@@ -4094,10 +4112,10 @@
         <v>1.4749380474017961E+18</v>
       </c>
       <c r="C98" t="s">
-        <v>401</v>
+        <v>456</v>
       </c>
       <c r="D98" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E98" s="2">
         <v>44556.208425925928</v>
@@ -4111,10 +4129,10 @@
         <v>1.474901587831177E+18</v>
       </c>
       <c r="C99" t="s">
-        <v>400</v>
+        <v>457</v>
       </c>
       <c r="D99" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E99" s="2">
         <v>44556.107812499999</v>
@@ -4128,10 +4146,10 @@
         <v>1.473726412473442E+18</v>
       </c>
       <c r="C100" t="s">
-        <v>399</v>
+        <v>458</v>
       </c>
       <c r="D100" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E100" s="2">
         <v>44552.864942129629</v>
@@ -4145,10 +4163,10 @@
         <v>1.473701054512521E+18</v>
       </c>
       <c r="C101" t="s">
-        <v>398</v>
+        <v>459</v>
       </c>
       <c r="D101" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E101" s="2">
         <v>44552.794976851852</v>
@@ -4179,7 +4197,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -4199,7 +4217,7 @@
         <v>1.496497589189022E+18</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2">
         <v>44615.701423611114</v>
@@ -4213,7 +4231,7 @@
         <v>1.496479736087958E+18</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D3" s="2">
         <v>44615.65215277778</v>
@@ -4227,7 +4245,7 @@
         <v>1.496462660124226E+18</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D4" s="2">
         <v>44615.605034722219</v>
@@ -4241,7 +4259,7 @@
         <v>1.496205536869728E+18</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D5" s="2">
         <v>44614.895509259259</v>
@@ -4255,7 +4273,7 @@
         <v>1.495619130669556E+18</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D6" s="2">
         <v>44613.277337962973</v>
@@ -4269,7 +4287,7 @@
         <v>1.4955983911113971E+18</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D7" s="2">
         <v>44613.220104166663</v>
@@ -4283,7 +4301,7 @@
         <v>1.4954265751727639E+18</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D8" s="2">
         <v>44612.745983796303</v>
@@ -4297,7 +4315,7 @@
         <v>1.493064014221431E+18</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D9" s="2">
         <v>44606.2265625</v>
@@ -4311,7 +4329,7 @@
         <v>1.4947228273118001E+18</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D10" s="2">
         <v>44610.804016203707</v>
@@ -4325,7 +4343,7 @@
         <v>1.4946563831443661E+18</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D11" s="2">
         <v>44610.620659722219</v>
@@ -4339,7 +4357,7 @@
         <v>1.494552860612256E+18</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D12" s="2">
         <v>44610.334999999999</v>
@@ -4353,7 +4371,7 @@
         <v>1.49431213538766E+18</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D13" s="2">
         <v>44609.670717592591</v>
@@ -4367,7 +4385,7 @@
         <v>1.494038005891445E+18</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D14" s="2">
         <v>44608.914270833331</v>
@@ -4381,7 +4399,7 @@
         <v>1.493679944546857E+18</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D15" s="2">
         <v>44607.926203703697</v>
@@ -4395,7 +4413,7 @@
         <v>1.4933134163999329E+18</v>
       </c>
       <c r="C16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D16" s="2">
         <v>44606.914780092593</v>
@@ -4409,7 +4427,7 @@
         <v>1.4932092611402921E+18</v>
       </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D17" s="2">
         <v>44606.62736111111</v>
@@ -4423,7 +4441,7 @@
         <v>1.4927544793678269E+18</v>
       </c>
       <c r="C18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D18" s="2">
         <v>44605.372407407413</v>
@@ -4451,7 +4469,7 @@
         <v>1.4921848652190021E+18</v>
       </c>
       <c r="C20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D20" s="2">
         <v>44603.800567129627</v>
@@ -4465,7 +4483,7 @@
         <v>1.492132092154626E+18</v>
       </c>
       <c r="C21" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D21" s="2">
         <v>44603.654942129629</v>
@@ -4479,7 +4497,7 @@
         <v>1.492113436976767E+18</v>
       </c>
       <c r="C22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D22" s="2">
         <v>44603.603472222218</v>
@@ -4493,7 +4511,7 @@
         <v>1.4920709015417411E+18</v>
       </c>
       <c r="C23" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D23" s="2">
         <v>44603.486087962963</v>
@@ -4507,7 +4525,7 @@
         <v>1.4920578290704881E+18</v>
       </c>
       <c r="C24" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D24" s="2">
         <v>44603.450023148151</v>
@@ -4521,7 +4539,7 @@
         <v>1.491436312951669E+18</v>
       </c>
       <c r="C25" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D25" s="2">
         <v>44601.734965277778</v>
@@ -4535,7 +4553,7 @@
         <v>1.4911970611692989E+18</v>
       </c>
       <c r="C26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D26" s="2">
         <v>44601.074756944443</v>
@@ -4549,7 +4567,7 @@
         <v>1.4910949816791199E+18</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D27" s="2">
         <v>44600.793067129627</v>
@@ -4563,7 +4581,7 @@
         <v>1.491016054327636E+18</v>
       </c>
       <c r="C28" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D28" s="2">
         <v>44600.575266203698</v>
@@ -4577,7 +4595,7 @@
         <v>1.4910125643563169E+18</v>
       </c>
       <c r="C29" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D29" s="2">
         <v>44600.565636574072</v>
@@ -4591,7 +4609,7 @@
         <v>1.4904666193987011E+18</v>
       </c>
       <c r="C30" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D30" s="2">
         <v>44599.059120370373</v>
@@ -4605,7 +4623,7 @@
         <v>1.4903946393917281E+18</v>
       </c>
       <c r="C31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D31" s="2">
         <v>44598.860486111109</v>
@@ -4619,7 +4637,7 @@
         <v>1.490325110905098E+18</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D32" s="2">
         <v>44598.668622685182</v>
@@ -4633,7 +4651,7 @@
         <v>1.490322862565122E+18</v>
       </c>
       <c r="C33" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D33" s="2">
         <v>44598.662418981483</v>
@@ -4647,7 +4665,7 @@
         <v>1.49013549454977E+18</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D34" s="2">
         <v>44598.145381944443</v>
@@ -4661,7 +4679,7 @@
         <v>1.490121458588213E+18</v>
       </c>
       <c r="C35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D35" s="2">
         <v>44598.10665509259</v>
@@ -4689,7 +4707,7 @@
         <v>1.433366270540386E+18</v>
       </c>
       <c r="C37" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D37" s="2">
         <v>44441.533842592587</v>
@@ -4703,7 +4721,7 @@
         <v>1.489008039596278E+18</v>
       </c>
       <c r="C38" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D38" s="2">
         <v>44595.034201388888</v>
@@ -4717,7 +4735,7 @@
         <v>1.4890004792124129E+18</v>
       </c>
       <c r="C39" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D39" s="2">
         <v>44595.013344907413</v>
@@ -4731,7 +4749,7 @@
         <v>1.4889945235061719E+18</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D40" s="2">
         <v>44594.99690972222</v>
@@ -4745,7 +4763,7 @@
         <v>1.4884793944862679E+18</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D41" s="2">
         <v>44593.575416666667</v>
@@ -4759,7 +4777,7 @@
         <v>1.487915151424725E+18</v>
       </c>
       <c r="C42" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D42" s="2">
         <v>44592.01840277778</v>
@@ -4773,7 +4791,7 @@
         <v>1.4879134019973079E+18</v>
       </c>
       <c r="C43" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D43" s="2">
         <v>44592.01357638889</v>
@@ -4787,7 +4805,7 @@
         <v>1.4876847100169869E+18</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D44" s="2">
         <v>44591.382511574076</v>
@@ -4801,7 +4819,7 @@
         <v>1.4874136059182001E+18</v>
       </c>
       <c r="C45" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D45" s="2">
         <v>44590.634409722217</v>
@@ -4815,7 +4833,7 @@
         <v>1.4869962274598871E+18</v>
       </c>
       <c r="C46" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D46" s="2">
         <v>44589.482662037037</v>
@@ -4829,7 +4847,7 @@
         <v>1.486751635573514E+18</v>
       </c>
       <c r="C47" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D47" s="2">
         <v>44588.807719907411</v>
@@ -4843,7 +4861,7 @@
         <v>1.4865907942365839E+18</v>
       </c>
       <c r="C48" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D48" s="2">
         <v>44588.363877314812</v>
@@ -4857,7 +4875,7 @@
         <v>1.486362281797632E+18</v>
       </c>
       <c r="C49" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D49" s="2">
         <v>44587.733298611107</v>
@@ -4871,7 +4889,7 @@
         <v>1.486302382766047E+18</v>
       </c>
       <c r="C50" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D50" s="2">
         <v>44587.568009259259</v>
@@ -4885,7 +4903,7 @@
         <v>1.4862169617344589E+18</v>
       </c>
       <c r="C51" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D51" s="2">
         <v>44587.332291666673</v>
@@ -4899,7 +4917,7 @@
         <v>1.486125885501673E+18</v>
       </c>
       <c r="C52" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D52" s="2">
         <v>44587.080972222233</v>
@@ -4913,7 +4931,7 @@
         <v>1.47200486262385E+18</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D53" s="2">
         <v>44548.114374999997</v>
@@ -4927,7 +4945,7 @@
         <v>1.4858464273393091E+18</v>
       </c>
       <c r="C54" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D54" s="2">
         <v>44586.309814814813</v>
@@ -4941,7 +4959,7 @@
         <v>1.4857284117546391E+18</v>
       </c>
       <c r="C55" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D55" s="2">
         <v>44585.984155092592</v>
@@ -4955,7 +4973,7 @@
         <v>1.4857203264284101E+18</v>
       </c>
       <c r="C56" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D56" s="2">
         <v>44585.961840277778</v>
@@ -4969,7 +4987,7 @@
         <v>1.4855368766185229E+18</v>
       </c>
       <c r="C57" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D57" s="2">
         <v>44585.455613425933</v>
@@ -4983,7 +5001,7 @@
         <v>1.5677588302844641E+18</v>
       </c>
       <c r="C58" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D58" s="2">
         <v>44812.386655092603</v>
@@ -4997,7 +5015,7 @@
         <v>1.484506180097655E+18</v>
       </c>
       <c r="C59" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D59" s="2">
         <v>44582.611435185187</v>
@@ -5011,7 +5029,7 @@
         <v>1.484430676657164E+18</v>
       </c>
       <c r="C60" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D60" s="2">
         <v>44582.403090277781</v>
@@ -5025,7 +5043,7 @@
         <v>1.4835632394222799E+18</v>
       </c>
       <c r="C61" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D61" s="2">
         <v>44580.009421296287</v>
@@ -5039,7 +5057,7 @@
         <v>1.4834345118536699E+18</v>
       </c>
       <c r="C62" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D62" s="2">
         <v>44579.65420138889</v>
@@ -5053,7 +5071,7 @@
         <v>1.483115891336352E+18</v>
       </c>
       <c r="C63" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D63" s="2">
         <v>44578.774976851862</v>
@@ -5067,7 +5085,7 @@
         <v>1.483088644411998E+18</v>
       </c>
       <c r="C64" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D64" s="2">
         <v>44578.699780092589</v>
@@ -5081,7 +5099,7 @@
         <v>1.482814735238242E+18</v>
       </c>
       <c r="C65" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D65" s="2">
         <v>44577.943935185183</v>
@@ -5095,7 +5113,7 @@
         <v>1.4825248905698801E+18</v>
       </c>
       <c r="C66" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D66" s="2">
         <v>44577.144120370373</v>
@@ -5109,7 +5127,7 @@
         <v>1.4825234506484979E+18</v>
       </c>
       <c r="C67" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D67" s="2">
         <v>44577.140150462961</v>
@@ -5123,7 +5141,7 @@
         <v>1.4825125147055099E+18</v>
       </c>
       <c r="C68" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D68" s="2">
         <v>44577.109965277778</v>
@@ -5137,7 +5155,7 @@
         <v>1.482454181701108E+18</v>
       </c>
       <c r="C69" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D69" s="2">
         <v>44576.949004629627</v>
@@ -5151,7 +5169,7 @@
         <v>1.482425824649396E+18</v>
       </c>
       <c r="C70" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D70" s="2">
         <v>44576.870752314811</v>
@@ -5165,7 +5183,7 @@
         <v>1.4819311112950661E+18</v>
       </c>
       <c r="C71" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D71" s="2">
         <v>44575.505601851852</v>
@@ -5193,7 +5211,7 @@
         <v>1.448482938979594E+18</v>
       </c>
       <c r="C73" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D73" s="2">
         <v>44483.247893518521</v>
@@ -5221,7 +5239,7 @@
         <v>1.4814368369165151E+18</v>
       </c>
       <c r="C75" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D75" s="2">
         <v>44574.14166666667</v>
@@ -5235,7 +5253,7 @@
         <v>1.4814352425734799E+18</v>
       </c>
       <c r="C76" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D76" s="2">
         <v>44574.13726851852</v>
@@ -5249,7 +5267,7 @@
         <v>1.4813921562585779E+18</v>
       </c>
       <c r="C77" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D77" s="2">
         <v>44574.018368055556</v>
@@ -5263,7 +5281,7 @@
         <v>1.4813882358174641E+18</v>
       </c>
       <c r="C78" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D78" s="2">
         <v>44574.0075462963</v>
@@ -5277,7 +5295,7 @@
         <v>1.480362152947028E+18</v>
       </c>
       <c r="C79" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D79" s="2">
         <v>44571.176099537042</v>
@@ -5291,7 +5309,7 @@
         <v>1.4803204688130619E+18</v>
       </c>
       <c r="C80" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D80" s="2">
         <v>44571.061076388891</v>
@@ -5305,7 +5323,7 @@
         <v>1.480310495781474E+18</v>
       </c>
       <c r="C81" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D81" s="2">
         <v>44571.033553240741</v>
@@ -5333,7 +5351,7 @@
         <v>1.479258790407115E+18</v>
       </c>
       <c r="C83" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D83" s="2">
         <v>44568.13140046296</v>
@@ -5347,7 +5365,7 @@
         <v>1.479118702964396E+18</v>
       </c>
       <c r="C84" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D84" s="2">
         <v>44567.744837962957</v>
@@ -5361,7 +5379,7 @@
         <v>1.479035678797279E+18</v>
       </c>
       <c r="C85" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D85" s="2">
         <v>44567.515729166669</v>
@@ -5375,7 +5393,7 @@
         <v>1.4787518093847219E+18</v>
       </c>
       <c r="C86" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D86" s="2">
         <v>44566.732395833344</v>
@@ -5389,7 +5407,7 @@
         <v>1.477658075737866E+18</v>
       </c>
       <c r="C87" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D87" s="2">
         <v>44563.714270833327</v>
@@ -5403,7 +5421,7 @@
         <v>1.47708230602845E+18</v>
       </c>
       <c r="C88" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D88" s="2">
         <v>44562.125451388893</v>
@@ -5417,7 +5435,7 @@
         <v>1.4770379770209121E+18</v>
       </c>
       <c r="C89" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D89" s="2">
         <v>44562.003125000003</v>
@@ -5431,7 +5449,7 @@
         <v>1.4770379754185851E+18</v>
       </c>
       <c r="C90" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D90" s="2">
         <v>44562.003125000003</v>
@@ -5445,7 +5463,7 @@
         <v>1.454360607726178E+18</v>
       </c>
       <c r="C91" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D91" s="2">
         <v>44499.467175925929</v>
@@ -5459,7 +5477,7 @@
         <v>1.476950490072162E+18</v>
       </c>
       <c r="C92" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D92" s="2">
         <v>44561.761701388888</v>
@@ -5473,7 +5491,7 @@
         <v>1.4769410577409679E+18</v>
       </c>
       <c r="C93" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D93" s="2">
         <v>44561.735682870371</v>
@@ -5487,7 +5505,7 @@
         <v>1.4769342083586911E+18</v>
       </c>
       <c r="C94" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D94" s="2">
         <v>44561.716782407413</v>
@@ -5501,7 +5519,7 @@
         <v>1.4758449438853161E+18</v>
       </c>
       <c r="C95" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D95" s="2">
         <v>44558.7109837963</v>
@@ -5515,7 +5533,7 @@
         <v>1.475129417219424E+18</v>
       </c>
       <c r="C96" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D96" s="2">
         <v>44556.736504629633</v>
@@ -5529,7 +5547,7 @@
         <v>1.4750229633008351E+18</v>
       </c>
       <c r="C97" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D97" s="2">
         <v>44556.442743055559</v>
@@ -5543,7 +5561,7 @@
         <v>1.4749380474017961E+18</v>
       </c>
       <c r="C98" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D98" s="2">
         <v>44556.208425925928</v>
@@ -5557,7 +5575,7 @@
         <v>1.474901587831177E+18</v>
       </c>
       <c r="C99" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D99" s="2">
         <v>44556.107812499999</v>
@@ -5571,7 +5589,7 @@
         <v>1.473726412473442E+18</v>
       </c>
       <c r="C100" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D100" s="2">
         <v>44552.864942129629</v>
@@ -5585,7 +5603,7 @@
         <v>1.473701054512521E+18</v>
       </c>
       <c r="C101" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D101" s="2">
         <v>44552.794976851852</v>
@@ -5603,25 +5621,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C69" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="58.85546875" customWidth="1"/>
     <col min="4" max="4" width="254.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -5638,10 +5657,10 @@
         <v>1.2593701393943759E+18</v>
       </c>
       <c r="C2" t="s">
-        <v>442</v>
+        <v>365</v>
       </c>
       <c r="D2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E2" s="2">
         <v>43961.395983796298</v>
@@ -5655,10 +5674,10 @@
         <v>1.262042767242519E+18</v>
       </c>
       <c r="C3" t="s">
-        <v>444</v>
+        <v>384</v>
       </c>
       <c r="D3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E3" s="2">
         <v>43968.77103009259</v>
@@ -5672,10 +5691,10 @@
         <v>1.2696541320356539E+18</v>
       </c>
       <c r="C4" t="s">
-        <v>445</v>
+        <v>367</v>
       </c>
       <c r="D4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E4" s="2">
         <v>43989.774398148147</v>
@@ -5689,7 +5708,7 @@
         <v>1.2731169314748211E+18</v>
       </c>
       <c r="D5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E5" s="2">
         <v>43999.329907407409</v>
@@ -5703,10 +5722,10 @@
         <v>1.2736061508193651E+18</v>
       </c>
       <c r="C6" t="s">
-        <v>446</v>
+        <v>471</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E6" s="2">
         <v>44000.679895833331</v>
@@ -5720,10 +5739,10 @@
         <v>1.2760779235570481E+18</v>
       </c>
       <c r="C7" t="s">
-        <v>447</v>
+        <v>472</v>
       </c>
       <c r="D7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E7" s="2">
         <v>44007.500694444447</v>
@@ -5737,7 +5756,7 @@
         <v>1.2763784237247731E+18</v>
       </c>
       <c r="D8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E8" s="2">
         <v>44008.329907407409</v>
@@ -5751,10 +5770,10 @@
         <v>1.2590681600550909E+18</v>
       </c>
       <c r="C9" t="s">
-        <v>448</v>
+        <v>368</v>
       </c>
       <c r="D9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E9" s="2">
         <v>43960.562685185178</v>
@@ -5768,7 +5787,7 @@
         <v>1.278551491108844E+18</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E10" s="2">
         <v>44014.326435185183</v>
@@ -5782,7 +5801,7 @@
         <v>1.2789138768857541E+18</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E11" s="2">
         <v>44015.326423611114</v>
@@ -5796,7 +5815,7 @@
         <v>1.2814506001196521E+18</v>
       </c>
       <c r="D12" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E12" s="2">
         <v>44022.32644675926</v>
@@ -5810,7 +5829,7 @@
         <v>1.282900142035735E+18</v>
       </c>
       <c r="D13" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E13" s="2">
         <v>44026.326423611114</v>
@@ -5824,7 +5843,7 @@
         <v>1.2836249157789E+18</v>
       </c>
       <c r="D14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E14" s="2">
         <v>44028.326423611114</v>
@@ -5838,10 +5857,10 @@
         <v>1.2865643788301481E+18</v>
       </c>
       <c r="C15" t="s">
-        <v>449</v>
+        <v>473</v>
       </c>
       <c r="D15" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E15" s="2">
         <v>44036.437789351847</v>
@@ -5855,7 +5874,7 @@
         <v>1.2891639366804851E+18</v>
       </c>
       <c r="D16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E16" s="2">
         <v>44043.611203703702</v>
@@ -5869,7 +5888,7 @@
         <v>1.292680835867595E+18</v>
       </c>
       <c r="D17" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E17" s="2">
         <v>44053.315995370373</v>
@@ -5883,10 +5902,10 @@
         <v>1.29465133464653E+18</v>
       </c>
       <c r="C18" t="s">
-        <v>449</v>
+        <v>473</v>
       </c>
       <c r="D18" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E18" s="2">
         <v>44058.753541666672</v>
@@ -5900,10 +5919,10 @@
         <v>1.2591184502340851E+18</v>
       </c>
       <c r="C19" t="s">
-        <v>450</v>
+        <v>369</v>
       </c>
       <c r="D19" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E19" s="2">
         <v>43960.701458333337</v>
@@ -5917,10 +5936,10 @@
         <v>1.3090348511363479E+18</v>
       </c>
       <c r="C20" t="s">
-        <v>451</v>
+        <v>474</v>
       </c>
       <c r="D20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E20" s="2">
         <v>44098.444479166668</v>
@@ -5934,10 +5953,10 @@
         <v>1.286931691450388E+18</v>
       </c>
       <c r="C21" t="s">
-        <v>452</v>
+        <v>475</v>
       </c>
       <c r="D21" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E21" s="2">
         <v>44037.451377314806</v>
@@ -5951,7 +5970,7 @@
         <v>1.313340720321909E+18</v>
       </c>
       <c r="D22" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E22" s="2">
         <v>44110.326423611114</v>
@@ -5965,7 +5984,7 @@
         <v>1.259709604243669E+18</v>
       </c>
       <c r="D23" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E23" s="2">
         <v>43962.332731481481</v>
@@ -5979,10 +5998,10 @@
         <v>1.2822836374347039E+18</v>
       </c>
       <c r="C24" t="s">
-        <v>453</v>
+        <v>370</v>
       </c>
       <c r="D24" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E24" s="2">
         <v>44024.625196759262</v>
@@ -5996,10 +6015,10 @@
         <v>1.3207709396934861E+18</v>
       </c>
       <c r="C25" t="s">
-        <v>454</v>
+        <v>476</v>
       </c>
       <c r="D25" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E25" s="2">
         <v>44130.788252314807</v>
@@ -6013,7 +6032,7 @@
         <v>1.260068462858326E+18</v>
       </c>
       <c r="D26" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E26" s="2">
         <v>43963.322997685187</v>
@@ -6027,10 +6046,10 @@
         <v>1.276784859235734E+18</v>
       </c>
       <c r="C27" t="s">
-        <v>455</v>
+        <v>477</v>
       </c>
       <c r="D27" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E27" s="2">
         <v>44009.451458333337</v>
@@ -6044,10 +6063,10 @@
         <v>1.330415730794377E+18</v>
       </c>
       <c r="C28" t="s">
-        <v>449</v>
+        <v>473</v>
       </c>
       <c r="D28" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E28" s="2">
         <v>44157.402800925927</v>
@@ -6061,10 +6080,10 @@
         <v>1.271059316770996E+18</v>
       </c>
       <c r="C29" t="s">
-        <v>456</v>
+        <v>478</v>
       </c>
       <c r="D29" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E29" s="2">
         <v>43993.651967592603</v>
@@ -6078,10 +6097,10 @@
         <v>1.260245777441599E+18</v>
       </c>
       <c r="C30" t="s">
-        <v>457</v>
+        <v>479</v>
       </c>
       <c r="D30" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E30" s="2">
         <v>43963.812291666669</v>
@@ -6095,7 +6114,7 @@
         <v>1.2604320938609869E+18</v>
       </c>
       <c r="D31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E31" s="2">
         <v>43964.326423611114</v>
@@ -6109,7 +6128,7 @@
         <v>1.2607944885171651E+18</v>
       </c>
       <c r="D32" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E32" s="2">
         <v>43965.32644675926</v>
@@ -6123,7 +6142,7 @@
         <v>1.266231560610562E+18</v>
       </c>
       <c r="D33" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E33" s="2">
         <v>43980.329907407409</v>
@@ -6137,10 +6156,10 @@
         <v>1.286932001342263E+18</v>
       </c>
       <c r="C34" t="s">
-        <v>458</v>
+        <v>480</v>
       </c>
       <c r="D34" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E34" s="2">
         <v>44037.452233796299</v>
@@ -6154,10 +6173,10 @@
         <v>1.3180945496344581E+18</v>
       </c>
       <c r="C35" t="s">
-        <v>443</v>
+        <v>366</v>
       </c>
       <c r="D35" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E35" s="2">
         <v>44123.444490740738</v>
@@ -6171,10 +6190,10 @@
         <v>1.3301201578349811E+18</v>
       </c>
       <c r="C36" t="s">
-        <v>459</v>
+        <v>371</v>
       </c>
       <c r="D36" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E36" s="2">
         <v>44156.587175925917</v>
@@ -6188,10 +6207,10 @@
         <v>1.356858718651113E+18</v>
       </c>
       <c r="C37" t="s">
-        <v>461</v>
+        <v>373</v>
       </c>
       <c r="D37" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E37" s="2">
         <v>44230.371550925927</v>
@@ -6205,7 +6224,7 @@
         <v>1.414993192739541E+18</v>
       </c>
       <c r="D38" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E38" s="2">
         <v>44390.833807870367</v>
@@ -6219,7 +6238,7 @@
         <v>1.435233914201719E+18</v>
       </c>
       <c r="D39" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E39" s="2">
         <v>44446.687557870369</v>
@@ -6233,10 +6252,10 @@
         <v>1.4706409089997371E+18</v>
       </c>
       <c r="C40" t="s">
-        <v>462</v>
+        <v>374</v>
       </c>
       <c r="D40" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E40" s="2">
         <v>44544.350578703707</v>
@@ -6250,7 +6269,7 @@
         <v>1.492820731339682E+18</v>
       </c>
       <c r="D41" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E41" s="2">
         <v>44605.555231481478</v>
@@ -6264,10 +6283,10 @@
         <v>1.262304156892778E+18</v>
       </c>
       <c r="C42" t="s">
-        <v>463</v>
+        <v>372</v>
       </c>
       <c r="D42" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E42" s="2">
         <v>43969.492337962962</v>
@@ -6281,10 +6300,10 @@
         <v>1.2731486275490691E+18</v>
       </c>
       <c r="C43" t="s">
-        <v>464</v>
+        <v>488</v>
       </c>
       <c r="D43" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E43" s="2">
         <v>43999.417372685188</v>
@@ -6298,10 +6317,10 @@
         <v>1.2854743306427231E+18</v>
       </c>
       <c r="C44" t="s">
-        <v>465</v>
+        <v>481</v>
       </c>
       <c r="D44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E44" s="2">
         <v>44033.429837962962</v>
@@ -6315,10 +6334,10 @@
         <v>1.286932244729344E+18</v>
       </c>
       <c r="C45" t="s">
-        <v>466</v>
+        <v>375</v>
       </c>
       <c r="D45" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E45" s="2">
         <v>44037.452905092592</v>
@@ -6332,7 +6351,7 @@
         <v>1.2905102865548979E+18</v>
       </c>
       <c r="D46" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E46" s="2">
         <v>44047.326423611114</v>
@@ -6346,10 +6365,10 @@
         <v>1.2964633217811991E+18</v>
       </c>
       <c r="C47" t="s">
-        <v>467</v>
+        <v>376</v>
       </c>
       <c r="D47" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E47" s="2">
         <v>44063.753668981481</v>
@@ -6363,10 +6382,10 @@
         <v>1.3117002232412119E+18</v>
       </c>
       <c r="C48" t="s">
-        <v>468</v>
+        <v>482</v>
       </c>
       <c r="D48" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E48" s="2">
         <v>44105.799513888887</v>
@@ -6380,10 +6399,10 @@
         <v>1.33981272340897E+18</v>
       </c>
       <c r="C49" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="D49" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E49" s="2">
         <v>44183.333564814813</v>
@@ -6397,7 +6416,7 @@
         <v>1.352207800408158E+18</v>
       </c>
       <c r="D50" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E50" s="2">
         <v>44217.537465277783</v>
@@ -6411,10 +6430,10 @@
         <v>1.3199075908774459E+18</v>
       </c>
       <c r="C51" t="s">
-        <v>470</v>
+        <v>377</v>
       </c>
       <c r="D51" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E51" s="2">
         <v>44128.447534722232</v>
@@ -6428,10 +6447,10 @@
         <v>1.4469058167627571E+18</v>
       </c>
       <c r="C52" t="s">
-        <v>471</v>
+        <v>378</v>
       </c>
       <c r="D52" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E52" s="2">
         <v>44478.895868055559</v>
@@ -6445,10 +6464,10 @@
         <v>1.3236599861452879E+18</v>
       </c>
       <c r="C53" t="s">
-        <v>472</v>
+        <v>379</v>
       </c>
       <c r="D53" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E53" s="2">
         <v>44138.760497685187</v>
@@ -6462,10 +6481,10 @@
         <v>1.477572892686975E+18</v>
       </c>
       <c r="C54" t="s">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="D54" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E54" s="2">
         <v>44563.479212962957</v>
@@ -6479,7 +6498,7 @@
         <v>1.491287008077132E+18</v>
       </c>
       <c r="D55" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E55" s="2">
         <v>44601.322962962957</v>
@@ -6493,7 +6512,7 @@
         <v>1.491650647984427E+18</v>
       </c>
       <c r="D56" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E56" s="2">
         <v>44602.326412037037</v>
@@ -6507,7 +6526,7 @@
         <v>1.4920130367391739E+18</v>
       </c>
       <c r="D57" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E57" s="2">
         <v>44603.326412037037</v>
@@ -6521,7 +6540,7 @@
         <v>1.4931035460442319E+18</v>
       </c>
       <c r="D58" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E58" s="2">
         <v>44606.335648148153</v>
@@ -6535,7 +6554,7 @@
         <v>1.4934625871530391E+18</v>
       </c>
       <c r="D59" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E59" s="2">
         <v>44607.326412037037</v>
@@ -6549,7 +6568,7 @@
         <v>1.493824975232406E+18</v>
       </c>
       <c r="D60" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E60" s="2">
         <v>44608.326412037037</v>
@@ -6563,7 +6582,7 @@
         <v>1.4941873601117061E+18</v>
       </c>
       <c r="D61" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E61" s="2">
         <v>44609.32640046296</v>
@@ -6577,10 +6596,10 @@
         <v>1.2601062137585129E+18</v>
       </c>
       <c r="C62" t="s">
-        <v>473</v>
+        <v>380</v>
       </c>
       <c r="D62" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E62" s="2">
         <v>43963.427164351851</v>
@@ -6594,7 +6613,7 @@
         <v>1.261155615386239E+18</v>
       </c>
       <c r="D63" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E63" s="2">
         <v>43966.322962962957</v>
@@ -6608,7 +6627,7 @@
         <v>1.2622490725529679E+18</v>
       </c>
       <c r="D64" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E64" s="2">
         <v>43969.34033564815</v>
@@ -6622,10 +6641,10 @@
         <v>1.2623472233225631E+18</v>
       </c>
       <c r="C65" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
       <c r="D65" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E65" s="2">
         <v>43969.611168981479</v>
@@ -6639,10 +6658,10 @@
         <v>1.262442993371529E+18</v>
       </c>
       <c r="C66" t="s">
-        <v>460</v>
+        <v>372</v>
       </c>
       <c r="D66" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E66" s="2">
         <v>43969.875451388893</v>
@@ -6656,7 +6675,7 @@
         <v>1.262605165254902E+18</v>
       </c>
       <c r="D67" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E67" s="2">
         <v>43970.322962962957</v>
@@ -6670,10 +6689,10 @@
         <v>1.262646747127562E+18</v>
       </c>
       <c r="C68" t="s">
-        <v>475</v>
+        <v>381</v>
       </c>
       <c r="D68" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E68" s="2">
         <v>43970.437708333331</v>
@@ -6687,10 +6706,10 @@
         <v>1.262770019949216E+18</v>
       </c>
       <c r="C69" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="D69" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E69" s="2">
         <v>43970.777870370373</v>
@@ -6704,7 +6723,7 @@
         <v>1.2629688115585229E+18</v>
       </c>
       <c r="D70" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E70" s="2">
         <v>43971.326435185183</v>
@@ -6718,7 +6737,7 @@
         <v>1.263331198220276E+18</v>
       </c>
       <c r="D71" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E71" s="2">
         <v>43972.326423611114</v>
@@ -6732,7 +6751,7 @@
         <v>1.26369358686609E+18</v>
       </c>
       <c r="D72" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E72" s="2">
         <v>43973.326435185183</v>
@@ -6746,10 +6765,10 @@
         <v>1.2638609770927549E+18</v>
       </c>
       <c r="C73" t="s">
-        <v>378</v>
+        <v>361</v>
       </c>
       <c r="D73" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E73" s="2">
         <v>43973.78833333333</v>
@@ -6763,10 +6782,10 @@
         <v>1.2640811703310541E+18</v>
       </c>
       <c r="C74" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="D74" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E74" s="2">
         <v>43974.395960648151</v>
@@ -6780,7 +6799,7 @@
         <v>1.264780749774954E+18</v>
       </c>
       <c r="D75" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E75" s="2">
         <v>43976.326423611114</v>
@@ -6794,7 +6813,7 @@
         <v>1.2648499612393549E+18</v>
       </c>
       <c r="D76" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E76" s="2">
         <v>43976.517418981479</v>
@@ -6808,7 +6827,7 @@
         <v>1.265143134406795E+18</v>
       </c>
       <c r="D77" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E77" s="2">
         <v>43977.326423611114</v>
@@ -6822,10 +6841,10 @@
         <v>1.265182159188439E+18</v>
       </c>
       <c r="C78" t="s">
-        <v>478</v>
+        <v>382</v>
       </c>
       <c r="D78" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E78" s="2">
         <v>43977.434108796297</v>
@@ -6839,10 +6858,10 @@
         <v>1.3272782488128141E+18</v>
       </c>
       <c r="C79" t="s">
-        <v>479</v>
+        <v>383</v>
       </c>
       <c r="D79" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E79" s="2">
         <v>44148.745000000003</v>
@@ -6856,7 +6875,7 @@
         <v>1.265505527406174E+18</v>
       </c>
       <c r="D80" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E80" s="2">
         <v>43978.326435185183</v>
@@ -6870,7 +6889,7 @@
         <v>1.2658691767464509E+18</v>
       </c>
       <c r="D81" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E81" s="2">
         <v>43979.329918981479</v>
@@ -6884,7 +6903,7 @@
         <v>1.2673174636891871E+18</v>
       </c>
       <c r="D82" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E82" s="2">
         <v>43983.326423611114</v>
@@ -6898,7 +6917,7 @@
         <v>1.267679850996937E+18</v>
       </c>
       <c r="D83" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E83" s="2">
         <v>43984.326423611114</v>
@@ -6912,7 +6931,7 @@
         <v>1.2680434993809039E+18</v>
       </c>
       <c r="D84" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E84" s="2">
         <v>43985.329907407409</v>
@@ -6926,7 +6945,7 @@
         <v>1.2684058861350221E+18</v>
       </c>
       <c r="D85" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E85" s="2">
         <v>43986.329895833333</v>
@@ -6940,7 +6959,7 @@
         <v>1.268768274629759E+18</v>
       </c>
       <c r="D86" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E86" s="2">
         <v>43987.329895833333</v>
@@ -6954,7 +6973,7 @@
         <v>1.26995235389936E+18</v>
       </c>
       <c r="D87" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E87" s="2">
         <v>43990.597337962958</v>
@@ -6968,7 +6987,7 @@
         <v>1.2702116048488161E+18</v>
       </c>
       <c r="D88" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E88" s="2">
         <v>43991.312731481477</v>
@@ -6982,10 +7001,10 @@
         <v>1.2703286074041549E+18</v>
       </c>
       <c r="C89" t="s">
-        <v>480</v>
+        <v>384</v>
       </c>
       <c r="D89" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E89" s="2">
         <v>43991.635601851849</v>
@@ -6999,7 +7018,7 @@
         <v>1.2705751779282371E+18</v>
       </c>
       <c r="D90" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E90" s="2">
         <v>43992.316006944442</v>
@@ -7013,7 +7032,7 @@
         <v>1.2709401002565839E+18</v>
       </c>
       <c r="D91" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E91" s="2">
         <v>43993.322997685187</v>
@@ -7027,10 +7046,10 @@
         <v>1.2709701653086369E+18</v>
       </c>
       <c r="C92" t="s">
-        <v>481</v>
+        <v>385</v>
       </c>
       <c r="D92" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E92" s="2">
         <v>43993.405960648153</v>
@@ -7044,10 +7063,10 @@
         <v>1.271004517421781E+18</v>
       </c>
       <c r="C93" t="s">
-        <v>482</v>
+        <v>386</v>
       </c>
       <c r="D93" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E93" s="2">
         <v>43993.500752314823</v>
@@ -7061,7 +7080,7 @@
         <v>1.2713024845317819E+18</v>
       </c>
       <c r="D94" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E94" s="2">
         <v>43994.32298611111</v>
@@ -7075,10 +7094,10 @@
         <v>1.2717745957297559E+18</v>
       </c>
       <c r="C95" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="D95" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E95" s="2">
         <v>43995.625763888893</v>
@@ -7092,10 +7111,10 @@
         <v>1.2720613426194839E+18</v>
       </c>
       <c r="C96" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="D96" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E96" s="2">
         <v>43996.417037037027</v>
@@ -7109,10 +7128,10 @@
         <v>1.2721040051965499E+18</v>
       </c>
       <c r="C97" t="s">
-        <v>484</v>
+        <v>387</v>
       </c>
       <c r="D97" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E97" s="2">
         <v>43996.534768518519</v>
@@ -7126,7 +7145,7 @@
         <v>1.2723883792048251E+18</v>
       </c>
       <c r="D98" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E98" s="2">
         <v>43997.319490740738</v>
@@ -7140,10 +7159,10 @@
         <v>1.272431292773216E+18</v>
       </c>
       <c r="C99" t="s">
-        <v>485</v>
+        <v>388</v>
       </c>
       <c r="D99" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E99" s="2">
         <v>43997.437905092593</v>
@@ -7157,7 +7176,7 @@
         <v>1.272752042709332E+18</v>
       </c>
       <c r="D100" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E100" s="2">
         <v>43998.323009259257</v>
@@ -7171,10 +7190,10 @@
         <v>1.2732573667299981E+18</v>
       </c>
       <c r="C101" t="s">
-        <v>486</v>
+        <v>389</v>
       </c>
       <c r="D101" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E101" s="2">
         <v>43999.717430555553</v>
@@ -7204,7 +7223,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -7224,7 +7243,7 @@
         <v>1.2593701393943759E+18</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D2" s="2">
         <v>43961.395983796298</v>
@@ -7238,7 +7257,7 @@
         <v>1.262042767242519E+18</v>
       </c>
       <c r="C3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D3" s="2">
         <v>43968.77103009259</v>
@@ -7252,7 +7271,7 @@
         <v>1.2696541320356539E+18</v>
       </c>
       <c r="C4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D4" s="2">
         <v>43989.774398148147</v>
@@ -7266,7 +7285,7 @@
         <v>1.2731169314748211E+18</v>
       </c>
       <c r="C5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D5" s="2">
         <v>43999.329907407409</v>
@@ -7280,7 +7299,7 @@
         <v>1.2736061508193651E+18</v>
       </c>
       <c r="C6" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D6" s="2">
         <v>44000.679895833331</v>
@@ -7294,7 +7313,7 @@
         <v>1.2760779235570481E+18</v>
       </c>
       <c r="C7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D7" s="2">
         <v>44007.500694444447</v>
@@ -7308,7 +7327,7 @@
         <v>1.2763784237247731E+18</v>
       </c>
       <c r="C8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D8" s="2">
         <v>44008.329907407409</v>
@@ -7322,7 +7341,7 @@
         <v>1.2590681600550909E+18</v>
       </c>
       <c r="C9" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D9" s="2">
         <v>43960.562685185178</v>
@@ -7336,7 +7355,7 @@
         <v>1.278551491108844E+18</v>
       </c>
       <c r="C10" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D10" s="2">
         <v>44014.326435185183</v>
@@ -7350,7 +7369,7 @@
         <v>1.2789138768857541E+18</v>
       </c>
       <c r="C11" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D11" s="2">
         <v>44015.326423611114</v>
@@ -7364,7 +7383,7 @@
         <v>1.2814506001196521E+18</v>
       </c>
       <c r="C12" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D12" s="2">
         <v>44022.32644675926</v>
@@ -7378,7 +7397,7 @@
         <v>1.282900142035735E+18</v>
       </c>
       <c r="C13" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D13" s="2">
         <v>44026.326423611114</v>
@@ -7392,7 +7411,7 @@
         <v>1.2836249157789E+18</v>
       </c>
       <c r="C14" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D14" s="2">
         <v>44028.326423611114</v>
@@ -7406,7 +7425,7 @@
         <v>1.2865643788301481E+18</v>
       </c>
       <c r="C15" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D15" s="2">
         <v>44036.437789351847</v>
@@ -7420,7 +7439,7 @@
         <v>1.2891639366804851E+18</v>
       </c>
       <c r="C16" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D16" s="2">
         <v>44043.611203703702</v>
@@ -7434,7 +7453,7 @@
         <v>1.292680835867595E+18</v>
       </c>
       <c r="C17" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D17" s="2">
         <v>44053.315995370373</v>
@@ -7448,7 +7467,7 @@
         <v>1.29465133464653E+18</v>
       </c>
       <c r="C18" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D18" s="2">
         <v>44058.753541666672</v>
@@ -7462,7 +7481,7 @@
         <v>1.2591184502340851E+18</v>
       </c>
       <c r="C19" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D19" s="2">
         <v>43960.701458333337</v>
@@ -7476,7 +7495,7 @@
         <v>1.3090348511363479E+18</v>
       </c>
       <c r="C20" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D20" s="2">
         <v>44098.444479166668</v>
@@ -7490,7 +7509,7 @@
         <v>1.286931691450388E+18</v>
       </c>
       <c r="C21" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D21" s="2">
         <v>44037.451377314806</v>
@@ -7504,7 +7523,7 @@
         <v>1.313340720321909E+18</v>
       </c>
       <c r="C22" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D22" s="2">
         <v>44110.326423611114</v>
@@ -7518,7 +7537,7 @@
         <v>1.259709604243669E+18</v>
       </c>
       <c r="C23" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D23" s="2">
         <v>43962.332731481481</v>
@@ -7532,7 +7551,7 @@
         <v>1.2822836374347039E+18</v>
       </c>
       <c r="C24" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D24" s="2">
         <v>44024.625196759262</v>
@@ -7546,7 +7565,7 @@
         <v>1.3207709396934861E+18</v>
       </c>
       <c r="C25" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D25" s="2">
         <v>44130.788252314807</v>
@@ -7560,7 +7579,7 @@
         <v>1.260068462858326E+18</v>
       </c>
       <c r="C26" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D26" s="2">
         <v>43963.322997685187</v>
@@ -7574,7 +7593,7 @@
         <v>1.276784859235734E+18</v>
       </c>
       <c r="C27" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D27" s="2">
         <v>44009.451458333337</v>
@@ -7588,7 +7607,7 @@
         <v>1.330415730794377E+18</v>
       </c>
       <c r="C28" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D28" s="2">
         <v>44157.402800925927</v>
@@ -7602,7 +7621,7 @@
         <v>1.271059316770996E+18</v>
       </c>
       <c r="C29" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D29" s="2">
         <v>43993.651967592603</v>
@@ -7616,7 +7635,7 @@
         <v>1.260245777441599E+18</v>
       </c>
       <c r="C30" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D30" s="2">
         <v>43963.812291666669</v>
@@ -7630,7 +7649,7 @@
         <v>1.2604320938609869E+18</v>
       </c>
       <c r="C31" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D31" s="2">
         <v>43964.326423611114</v>
@@ -7644,7 +7663,7 @@
         <v>1.2607944885171651E+18</v>
       </c>
       <c r="C32" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D32" s="2">
         <v>43965.32644675926</v>
@@ -7658,7 +7677,7 @@
         <v>1.266231560610562E+18</v>
       </c>
       <c r="C33" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D33" s="2">
         <v>43980.329907407409</v>
@@ -7672,7 +7691,7 @@
         <v>1.286932001342263E+18</v>
       </c>
       <c r="C34" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D34" s="2">
         <v>44037.452233796299</v>
@@ -7686,7 +7705,7 @@
         <v>1.3180945496344581E+18</v>
       </c>
       <c r="C35" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D35" s="2">
         <v>44123.444490740738</v>
@@ -7700,7 +7719,7 @@
         <v>1.3301201578349811E+18</v>
       </c>
       <c r="C36" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D36" s="2">
         <v>44156.587175925917</v>
@@ -7714,7 +7733,7 @@
         <v>1.356858718651113E+18</v>
       </c>
       <c r="C37" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D37" s="2">
         <v>44230.371550925927</v>
@@ -7728,7 +7747,7 @@
         <v>1.414993192739541E+18</v>
       </c>
       <c r="C38" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D38" s="2">
         <v>44390.833807870367</v>
@@ -7742,7 +7761,7 @@
         <v>1.435233914201719E+18</v>
       </c>
       <c r="C39" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D39" s="2">
         <v>44446.687557870369</v>
@@ -7756,7 +7775,7 @@
         <v>1.4706409089997371E+18</v>
       </c>
       <c r="C40" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D40" s="2">
         <v>44544.350578703707</v>
@@ -7770,7 +7789,7 @@
         <v>1.492820731339682E+18</v>
       </c>
       <c r="C41" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D41" s="2">
         <v>44605.555231481478</v>
@@ -7784,7 +7803,7 @@
         <v>1.262304156892778E+18</v>
       </c>
       <c r="C42" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D42" s="2">
         <v>43969.492337962962</v>
@@ -7798,7 +7817,7 @@
         <v>1.2731486275490691E+18</v>
       </c>
       <c r="C43" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D43" s="2">
         <v>43999.417372685188</v>
@@ -7812,7 +7831,7 @@
         <v>1.2854743306427231E+18</v>
       </c>
       <c r="C44" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D44" s="2">
         <v>44033.429837962962</v>
@@ -7826,7 +7845,7 @@
         <v>1.286932244729344E+18</v>
       </c>
       <c r="C45" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D45" s="2">
         <v>44037.452905092592</v>
@@ -7840,7 +7859,7 @@
         <v>1.2905102865548979E+18</v>
       </c>
       <c r="C46" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D46" s="2">
         <v>44047.326423611114</v>
@@ -7854,7 +7873,7 @@
         <v>1.2964633217811991E+18</v>
       </c>
       <c r="C47" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D47" s="2">
         <v>44063.753668981481</v>
@@ -7868,7 +7887,7 @@
         <v>1.3117002232412119E+18</v>
       </c>
       <c r="C48" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D48" s="2">
         <v>44105.799513888887</v>
@@ -7882,7 +7901,7 @@
         <v>1.33981272340897E+18</v>
       </c>
       <c r="C49" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D49" s="2">
         <v>44183.333564814813</v>
@@ -7896,7 +7915,7 @@
         <v>1.352207800408158E+18</v>
       </c>
       <c r="C50" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D50" s="2">
         <v>44217.537465277783</v>
@@ -7910,7 +7929,7 @@
         <v>1.3199075908774459E+18</v>
       </c>
       <c r="C51" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D51" s="2">
         <v>44128.447534722232</v>
@@ -7924,7 +7943,7 @@
         <v>1.4469058167627571E+18</v>
       </c>
       <c r="C52" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D52" s="2">
         <v>44478.895868055559</v>
@@ -7938,7 +7957,7 @@
         <v>1.3236599861452879E+18</v>
       </c>
       <c r="C53" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D53" s="2">
         <v>44138.760497685187</v>
@@ -7952,7 +7971,7 @@
         <v>1.477572892686975E+18</v>
       </c>
       <c r="C54" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D54" s="2">
         <v>44563.479212962957</v>
@@ -7966,7 +7985,7 @@
         <v>1.491287008077132E+18</v>
       </c>
       <c r="C55" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D55" s="2">
         <v>44601.322962962957</v>
@@ -7980,7 +7999,7 @@
         <v>1.491650647984427E+18</v>
       </c>
       <c r="C56" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D56" s="2">
         <v>44602.326412037037</v>
@@ -7994,7 +8013,7 @@
         <v>1.4920130367391739E+18</v>
       </c>
       <c r="C57" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D57" s="2">
         <v>44603.326412037037</v>
@@ -8008,7 +8027,7 @@
         <v>1.4931035460442319E+18</v>
       </c>
       <c r="C58" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D58" s="2">
         <v>44606.335648148153</v>
@@ -8022,7 +8041,7 @@
         <v>1.4934625871530391E+18</v>
       </c>
       <c r="C59" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D59" s="2">
         <v>44607.326412037037</v>
@@ -8036,7 +8055,7 @@
         <v>1.493824975232406E+18</v>
       </c>
       <c r="C60" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D60" s="2">
         <v>44608.326412037037</v>
@@ -8050,7 +8069,7 @@
         <v>1.4941873601117061E+18</v>
       </c>
       <c r="C61" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D61" s="2">
         <v>44609.32640046296</v>
@@ -8064,7 +8083,7 @@
         <v>1.2601062137585129E+18</v>
       </c>
       <c r="C62" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D62" s="2">
         <v>43963.427164351851</v>
@@ -8078,7 +8097,7 @@
         <v>1.261155615386239E+18</v>
       </c>
       <c r="C63" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D63" s="2">
         <v>43966.322962962957</v>
@@ -8092,7 +8111,7 @@
         <v>1.2622490725529679E+18</v>
       </c>
       <c r="C64" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D64" s="2">
         <v>43969.34033564815</v>
@@ -8106,7 +8125,7 @@
         <v>1.2623472233225631E+18</v>
       </c>
       <c r="C65" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D65" s="2">
         <v>43969.611168981479</v>
@@ -8120,7 +8139,7 @@
         <v>1.262442993371529E+18</v>
       </c>
       <c r="C66" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D66" s="2">
         <v>43969.875451388893</v>
@@ -8134,7 +8153,7 @@
         <v>1.262605165254902E+18</v>
       </c>
       <c r="C67" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D67" s="2">
         <v>43970.322962962957</v>
@@ -8148,7 +8167,7 @@
         <v>1.262646747127562E+18</v>
       </c>
       <c r="C68" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D68" s="2">
         <v>43970.437708333331</v>
@@ -8162,7 +8181,7 @@
         <v>1.262770019949216E+18</v>
       </c>
       <c r="C69" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D69" s="2">
         <v>43970.777870370373</v>
@@ -8176,7 +8195,7 @@
         <v>1.2629688115585229E+18</v>
       </c>
       <c r="C70" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D70" s="2">
         <v>43971.326435185183</v>
@@ -8190,7 +8209,7 @@
         <v>1.263331198220276E+18</v>
       </c>
       <c r="C71" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D71" s="2">
         <v>43972.326423611114</v>
@@ -8204,7 +8223,7 @@
         <v>1.26369358686609E+18</v>
       </c>
       <c r="C72" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D72" s="2">
         <v>43973.326435185183</v>
@@ -8218,7 +8237,7 @@
         <v>1.2638609770927549E+18</v>
       </c>
       <c r="C73" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D73" s="2">
         <v>43973.78833333333</v>
@@ -8232,7 +8251,7 @@
         <v>1.2640811703310541E+18</v>
       </c>
       <c r="C74" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D74" s="2">
         <v>43974.395960648151</v>
@@ -8246,7 +8265,7 @@
         <v>1.264780749774954E+18</v>
       </c>
       <c r="C75" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D75" s="2">
         <v>43976.326423611114</v>
@@ -8260,7 +8279,7 @@
         <v>1.2648499612393549E+18</v>
       </c>
       <c r="C76" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D76" s="2">
         <v>43976.517418981479</v>
@@ -8274,7 +8293,7 @@
         <v>1.265143134406795E+18</v>
       </c>
       <c r="C77" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D77" s="2">
         <v>43977.326423611114</v>
@@ -8288,7 +8307,7 @@
         <v>1.265182159188439E+18</v>
       </c>
       <c r="C78" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D78" s="2">
         <v>43977.434108796297</v>
@@ -8302,7 +8321,7 @@
         <v>1.3272782488128141E+18</v>
       </c>
       <c r="C79" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D79" s="2">
         <v>44148.745000000003</v>
@@ -8316,7 +8335,7 @@
         <v>1.265505527406174E+18</v>
       </c>
       <c r="C80" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D80" s="2">
         <v>43978.326435185183</v>
@@ -8330,7 +8349,7 @@
         <v>1.2658691767464509E+18</v>
       </c>
       <c r="C81" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D81" s="2">
         <v>43979.329918981479</v>
@@ -8344,7 +8363,7 @@
         <v>1.2673174636891871E+18</v>
       </c>
       <c r="C82" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D82" s="2">
         <v>43983.326423611114</v>
@@ -8358,7 +8377,7 @@
         <v>1.267679850996937E+18</v>
       </c>
       <c r="C83" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D83" s="2">
         <v>43984.326423611114</v>
@@ -8372,7 +8391,7 @@
         <v>1.2680434993809039E+18</v>
       </c>
       <c r="C84" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D84" s="2">
         <v>43985.329907407409</v>
@@ -8386,7 +8405,7 @@
         <v>1.2684058861350221E+18</v>
       </c>
       <c r="C85" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D85" s="2">
         <v>43986.329895833333</v>
@@ -8400,7 +8419,7 @@
         <v>1.268768274629759E+18</v>
       </c>
       <c r="C86" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D86" s="2">
         <v>43987.329895833333</v>
@@ -8414,7 +8433,7 @@
         <v>1.26995235389936E+18</v>
       </c>
       <c r="C87" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D87" s="2">
         <v>43990.597337962958</v>
@@ -8428,7 +8447,7 @@
         <v>1.2702116048488161E+18</v>
       </c>
       <c r="C88" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D88" s="2">
         <v>43991.312731481477</v>
@@ -8442,7 +8461,7 @@
         <v>1.2703286074041549E+18</v>
       </c>
       <c r="C89" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D89" s="2">
         <v>43991.635601851849</v>
@@ -8456,7 +8475,7 @@
         <v>1.2705751779282371E+18</v>
       </c>
       <c r="C90" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D90" s="2">
         <v>43992.316006944442</v>
@@ -8470,7 +8489,7 @@
         <v>1.2709401002565839E+18</v>
       </c>
       <c r="C91" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D91" s="2">
         <v>43993.322997685187</v>
@@ -8484,7 +8503,7 @@
         <v>1.2709701653086369E+18</v>
       </c>
       <c r="C92" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D92" s="2">
         <v>43993.405960648153</v>
@@ -8498,7 +8517,7 @@
         <v>1.271004517421781E+18</v>
       </c>
       <c r="C93" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D93" s="2">
         <v>43993.500752314823</v>
@@ -8512,7 +8531,7 @@
         <v>1.2713024845317819E+18</v>
       </c>
       <c r="C94" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D94" s="2">
         <v>43994.32298611111</v>
@@ -8526,7 +8545,7 @@
         <v>1.2717745957297559E+18</v>
       </c>
       <c r="C95" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D95" s="2">
         <v>43995.625763888893</v>
@@ -8540,7 +8559,7 @@
         <v>1.2720613426194839E+18</v>
       </c>
       <c r="C96" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D96" s="2">
         <v>43996.417037037027</v>
@@ -8554,7 +8573,7 @@
         <v>1.2721040051965499E+18</v>
       </c>
       <c r="C97" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D97" s="2">
         <v>43996.534768518519</v>
@@ -8568,7 +8587,7 @@
         <v>1.2723883792048251E+18</v>
       </c>
       <c r="C98" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D98" s="2">
         <v>43997.319490740738</v>
@@ -8582,7 +8601,7 @@
         <v>1.272431292773216E+18</v>
       </c>
       <c r="C99" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D99" s="2">
         <v>43997.437905092593</v>
@@ -8596,7 +8615,7 @@
         <v>1.272752042709332E+18</v>
       </c>
       <c r="C100" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D100" s="2">
         <v>43998.323009259257</v>
@@ -8610,7 +8629,7 @@
         <v>1.2732573667299981E+18</v>
       </c>
       <c r="C101" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D101" s="2">
         <v>43999.717430555553</v>

</xml_diff>

<commit_message>
Changes to words of interest calculation with regex algorithm
</commit_message>
<xml_diff>
--- a/server/tests/tweets.xlsx
+++ b/server/tests/tweets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="pyrosvestiki" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="490">
   <si>
     <t>id</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t xml:space="preserve">Δ.T. σχετικά με την επιχείρηση στην περιοχή Ύδατα Στυγός πλησίον του χιονοδρομικού κέντρου Καλαβρύτων   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Σε ασφαλές σημείο μεταφέρθηκε ένα σκυλάκι μετά  από πτώση του σε δύσβατο σημείο, στην περιοχή  Άγιος Στέφανος Αυλιωτών Κέρκυρας. Επιχείρησαν 2 πυροσβέστες με 1 όχημα. Συνδρομή της εθελοντικής ομάδας Ε.Μ.Ε.Δ. Κέρκυρας. </t>
   </si>
   <si>
     <t>Σε συνέχεια προηγούμενων μηνυμάτων, χωρίς αισθήσεις εντοπίστηκε και τρίτος άνδρας στην περιοχή Ύδατα Στυγός πλησίον του χιονοδρομικού κέντρου Καλαβρύτων. Σε εξέλιξη η επιχείρηση μεταφοράς και των τριών απο δυνάμεις του Π.Σ. και της Ο.Ε.Δ.</t>
@@ -285,10 +282,6 @@
 Επιχείρησαν 11 πυροσβέστες με 4 οχήματα.</t>
   </si>
   <si>
-    <t>Τραυματισμένος απεγκλωβίστηκε και παραδόθηκε στο ΕΚΑΒ, ένας άνδρας, συνεπεία τροχαίου, ύστερα από σύγκρουση με έτερο ΕΙΧ όχημα, επί της Επ. οδού Σιάτοστας  Κνίδης στο Δήμο Βοΐου, Κοζάνης.
-Επιχείρησαν 5 πυροσβέστες με 1 όχημα.</t>
-  </si>
-  <si>
     <t>Κατεσβέσθη πυρκαγιά σε σταθμευμένο ΕΙΧ όχημα στη συμβολή των οδών Συνταγματάρχου Δαβάκη και Σοφοκλέους στην Καλλιθέα Αττικής. 
 Επιχείρησαν 6 πυροσβέστες με 2 οχήματα.</t>
   </si>
@@ -309,10 +302,6 @@
   <si>
     <t>Ολοκληρώθηκε η κατάσβεση πυρκαγιάς σε εγκαταλελειμμένο  σιδηροδρομικό βαγόνι στη Λάρισα. 
 Επιχείρησαν 7 πυροσβέστες με 3 οχήματα.</t>
-  </si>
-  <si>
-    <t>Σορός ατόμου εντοπίστηκε κατά τη διάρκεια κατάσβεσης πυρκαγιάς σε ΕΙΧ όχημα στην Ε.Ο. Χρυσοπηγής  Λακκωμάτων στο δήμο Φαρρών Αχαΐας.
-Επιχειρούν  8 πυροσβέστες με 3 οχήματα.</t>
   </si>
   <si>
     <t xml:space="preserve">Καμία διατάραξη της λειτουργίας του Πυροσβεστικού Σώματος εξαιτίας της πανδημίας.
@@ -1392,9 +1381,6 @@
     <t>ΠαιδοΟγκολογικής Κλινικής ΠαΓΝΗ Κρήτης</t>
   </si>
   <si>
-    <t>Δ.Ε. Λιβαδίου Ελασσόνας της Π.Ε. Λάρισας</t>
-  </si>
-  <si>
     <t>Λαμία</t>
   </si>
   <si>
@@ -1404,12 +1390,6 @@
     <t>Μυτιλήνη</t>
   </si>
   <si>
-    <t>Γράμμου Καστοριάς</t>
-  </si>
-  <si>
-    <t>Αρκαδίας Κορινθίας</t>
-  </si>
-  <si>
     <t>Γεράνια Όρη</t>
   </si>
   <si>
@@ -1428,9 +1408,6 @@
     <t>Λ. Μαρκοπούλου</t>
   </si>
   <si>
-    <t>Δήμου Αθηναίων</t>
-  </si>
-  <si>
     <t>Λ. Κατεχάκη</t>
   </si>
   <si>
@@ -1458,205 +1435,19 @@
     <t>Καλλιθέα</t>
   </si>
   <si>
-    <t>Μαγνησίας</t>
-  </si>
-  <si>
-    <t>Στερεάς Ελλάδας</t>
-  </si>
-  <si>
-    <t>Κοζάνης</t>
-  </si>
-  <si>
     <t>Κέρκυρα</t>
   </si>
   <si>
     <t>λίμνη Περδίκκα Πτολεμαΐδας</t>
   </si>
   <si>
-    <t>στο Κρυονέρι Αττικής</t>
-  </si>
-  <si>
-    <t>επί της Αποστόλου Παύλου στη Θεσσαλονίκη</t>
-  </si>
-  <si>
-    <t>επί της οδού Σόλωνος στη Μενεμένη Θεσσαλονίκης</t>
-  </si>
-  <si>
-    <t>επί της οδού Ιβήρων στην Αθήνα</t>
-  </si>
-  <si>
     <t>Π.Υ. Ρεθύμνου</t>
-  </si>
-  <si>
-    <t>επί της οδού Μύρων στην Αθήνα</t>
-  </si>
-  <si>
-    <t>στην περιοχή Γούμερο νομού Ηλείας</t>
-  </si>
-  <si>
-    <t>κοινότητα Πάλιουρα στο δήμο Διρφύων Μεσσαπίων Ευβοίας</t>
-  </si>
-  <si>
-    <t>στην Κρήτη</t>
-  </si>
-  <si>
-    <t>Φαράγγι της Γκούρας στη Φυλή Αττικής</t>
-  </si>
-  <si>
-    <t>στην Δραπετσώνα</t>
-  </si>
-  <si>
-    <t>στην Καστέλλα Πειραιώς</t>
-  </si>
-  <si>
-    <t>επί της οδού Ελευθερίου Βενιζέλου στον Πειραιά</t>
-  </si>
-  <si>
-    <t>στη Δραπετσώνα</t>
-  </si>
-  <si>
-    <t>στο Διεθνή Αερολιμένα Αθηνών</t>
-  </si>
-  <si>
-    <t>επί της οδού Μ. Αλεξάνδρου στο δήμο Θέρμης Θεσσαλονίκης</t>
-  </si>
-  <si>
-    <t>στο δήμο Κατερίνης Πιερίας</t>
-  </si>
-  <si>
-    <t>στο Αιγάλεω</t>
-  </si>
-  <si>
-    <t>επί των οδών Θηβών και Πέτρου Ράλλη στο Αιγάλεω Αττικής</t>
-  </si>
-  <si>
-    <t>στην περιοχή Άγιος Στέφανος Αυλιωτών Κέρκυρας</t>
-  </si>
-  <si>
-    <t>των οδών Χαριλάου Τρικούπη και Ναυαρίνου στο δήμο Αθηναίων Αττικής</t>
-  </si>
-  <si>
-    <t>επί της οδού Σαμαρίνας στο δήμο Αχαρνών Αττικής</t>
-  </si>
-  <si>
-    <t>στην περιοχή Λιχάδα Ευβοίας</t>
-  </si>
-  <si>
-    <t>δημοτική κοινότητα Φύλλου του δήμου Παλαμά Καρδίτσας</t>
-  </si>
-  <si>
-    <t>δημοτική κοινότητα Ιαλυσού της Ρόδου</t>
-  </si>
-  <si>
-    <t>στην περιοχή Μαράσια Έβρου</t>
-  </si>
-  <si>
-    <t>δασάκι Κουτσουρά του δήμου Ιεράπετρας</t>
-  </si>
-  <si>
-    <t>επί της Λεωφόρου Δημοκρατίας στο Κερατσίνι Αττικής</t>
-  </si>
-  <si>
-    <t>επί της οδού 17ης Οκτωβρίου στη Νάουσα Ημαθίας</t>
-  </si>
-  <si>
-    <t>στο Υπουργείο Κλιματικής Κρίσης</t>
-  </si>
-  <si>
-    <t>επί της οδού Εσπερίδων στη Κηφισιά</t>
-  </si>
-  <si>
-    <t>στην Αττική</t>
-  </si>
-  <si>
-    <t>στην περιοχή Βασιλική Λευκάδας</t>
-  </si>
-  <si>
-    <t>επί της Λ. Συγγρού στην Αθήνα</t>
-  </si>
-  <si>
-    <t>επί της οδού Σεράφη στο Αθηναίων</t>
-  </si>
-  <si>
-    <t>στην περιοχή Δαύλειας στη Λιβαδειά Βοιωτίας</t>
-  </si>
-  <si>
-    <t>επί της οδού Άνδρου στο Κορωπί</t>
-  </si>
-  <si>
-    <t>στο Μαρούσι στο Διακοπτό Αχαΐας</t>
-  </si>
-  <si>
-    <t>επί της οδού Κυπρίων Αγωνιστών στο Μαρούσι Αττικής</t>
-  </si>
-  <si>
-    <t>επί της οδού Λευκάδας στο Κορωπί</t>
-  </si>
-  <si>
-    <t>επί της οδού Αναξάρχου στο δήμο της Ξάνθης</t>
-  </si>
-  <si>
-    <t>στη Νέα Ποτίδαια Χαλκιδικής</t>
-  </si>
-  <si>
-    <t>στην περιοχή Μάραθος στο Ηράκλειο Κρήτης</t>
-  </si>
-  <si>
-    <t>επί της οδού Αγρινίου στο δήμο Πεύκης Αττικής</t>
-  </si>
-  <si>
-    <t>επί της οδού Πάφου στο δήμο Αμαρουσίου Αττικής</t>
-  </si>
-  <si>
-    <t>στην Ε.Ο. ΑθηνώνΚορίνθου στην Κακιά Σκάλα Μεγάρων Σήραγγα Ευπαλίνος</t>
-  </si>
-  <si>
-    <t>στην περιοχή Καθαρό Λασιθίου</t>
-  </si>
-  <si>
-    <t>επί της οδού Αγίου Μελετίου στην Αθήνα</t>
-  </si>
-  <si>
-    <t>επί της οδού Νικήτα στον Πειραιά</t>
-  </si>
-  <si>
-    <t>επί της οδού Κωννου Παλαιολόγου στη Νέα Ερυθραία Αττικής</t>
-  </si>
-  <si>
-    <t>επί της οδού Μονής Πετράκη στην Αθήνα</t>
-  </si>
-  <si>
-    <t>στον Ασπρόπυργο Αττικής</t>
-  </si>
-  <si>
-    <t>στη συμβολή των οδών Συνταγματάρχου Δαβάκη και Σοφοκλέους στην Καλλιθέα Αττικής</t>
-  </si>
-  <si>
-    <t>επί της οδού Ελ. Βενιζέλου στο Πέραμα Αττικής</t>
-  </si>
-  <si>
-    <t>στην περιοχή Πλατύ δήμου Αλεξάνδρειας Ημαθίας</t>
-  </si>
-  <si>
-    <t>στη Λάρισα</t>
-  </si>
-  <si>
-    <t>στη συμβολή των οδών Γαλήνης και Ρόδων στην Εκάλη Αττικής</t>
   </si>
   <si>
     <t>Απεγκλωβίστηκε μια γυναίκα από ΕΙΧ όχημα, συνεπεία τροχαίου, ύστερα από σύγκρουση με έτερο όχημα, πλησίον του κόμβου Δωρικού επί της Ε.Ο. Αλεξανδρούπολης ΒΙ.ΠΕ Αλεξανδρούπολης, Έβρου.
 Επιχείρησαν 4 πυροσβέστες με 2 οχήματα.</t>
   </si>
   <si>
-    <t>κόμβου Δωρικού επί της Ε.Ο. Αλεξανδρούπολης ΒΙ.ΠΕ Αλεξανδρούπολης Έβρου</t>
-  </si>
-  <si>
-    <t>επί της οδού Στρατάρχου Αλεξάνδρου Παπάγου στον Εύοσμο Θεσσαλονίκης</t>
-  </si>
-  <si>
-    <t>την Πυροσβεστική Υπηρεσία Διεθνούς Αερολιμένα Αθηνών Ελευθέριος Βενιζέλος</t>
-  </si>
-  <si>
     <t xml:space="preserve">12.598 στελέχη υπηρεσιών έλαβαν πιστοποιημένη εκπαίδευση από την Πυροσβεστική Υπηρεσία Διεθνούς Αερολιμένα Αθηνών Ελευθέριος Βενιζέλος.
 Σχετικό Δελτίο Τύπου θα βρείτε  </t>
   </si>
@@ -1664,60 +1455,9 @@
     <t>Ολοκληρώθηκε η επιχείρηση ανεύρεσης άνδρα στην περιοχή Χρυσοκελλαριά, του δήμου Πύλου Νέστορος, όπου και παρελήφθη από ασθενοφόρο του ΕΚΑΒ για προληπτικούς λόγους.</t>
   </si>
   <si>
-    <t>στην περιοχή Χρυσοκελλαριά του δήμου Πύλου Νέστορος</t>
-  </si>
-  <si>
-    <t>επί της οδού Καλλέργη στην Αθήνα</t>
-  </si>
-  <si>
-    <t>στην περιοχή επάνω Χερσόνησος του δήμου Χερσονήσου Κρήτης</t>
-  </si>
-  <si>
-    <t>επί της Λεωφόρου Μαραθώνος στη Νέα Μάκρη Αττικής</t>
-  </si>
-  <si>
-    <t>επί της οδού Ελασιδών στην Αθήνα</t>
-  </si>
-  <si>
-    <t>επί της οδού Αγ. Φωτεινής στη Ν. Σμύρνη Αττικής</t>
-  </si>
-  <si>
     <t>νήσου Ερεικούσας</t>
   </si>
   <si>
-    <t>επί της οδού Κωστή Παλαμά στη Δραπετσώνα</t>
-  </si>
-  <si>
-    <t>στη Λευκίμμη Κέρκυρας</t>
-  </si>
-  <si>
-    <t>επί της οδού 3ης Σεπτεμβρίου στην Αθήνα</t>
-  </si>
-  <si>
-    <t>στην περιοχή Ύδατα Στυγός</t>
-  </si>
-  <si>
-    <t>στη Νάουσα Ημαθίας</t>
-  </si>
-  <si>
-    <t>δημοτική κοινότητα Πεταλούδων της Ρόδου</t>
-  </si>
-  <si>
-    <t>στην ορεινή περιοχή Θεοδωριανά Άρτας</t>
-  </si>
-  <si>
-    <t>επί της Επ. οδού Σιάτοστας Κνίδης στο Δήμο Βοΐου Κοζάνης</t>
-  </si>
-  <si>
-    <t>Ε.Ο. Χρυσοπηγής Λακκωμάτων Φαρρών Αχαΐας</t>
-  </si>
-  <si>
-    <t>επί της οδού Ν. Παπαδημητρίου στα Καμένα Βούρλα Φθιωτιδας</t>
-  </si>
-  <si>
-    <t>Καβάλας Ξάνθης</t>
-  </si>
-  <si>
     <t>Ημαθίας</t>
   </si>
   <si>
@@ -1727,15 +1467,9 @@
     <t>Πέραμα Αττικής</t>
   </si>
   <si>
-    <t>Λιοσίων</t>
-  </si>
-  <si>
     <t>Θρακομακεδόνες</t>
   </si>
   <si>
-    <t>Θεσσαλονίκης</t>
-  </si>
-  <si>
     <t>Λ. Αθηνών</t>
   </si>
   <si>
@@ -1745,9 +1479,6 @@
     <t>Λ. Μεσογείων</t>
   </si>
   <si>
-    <t>Δεκελείας Κηφισιά</t>
-  </si>
-  <si>
     <t>Αθήνας</t>
   </si>
   <si>
@@ -1760,13 +1491,285 @@
     <t>Αρτέμιδα</t>
   </si>
   <si>
-    <t>Γλυφάδας</t>
-  </si>
-  <si>
-    <t>Πρέβεζας</t>
-  </si>
-  <si>
-    <t>Φθιώτιδας</t>
+    <t>Κρυονέρι Αττικής</t>
+  </si>
+  <si>
+    <t>περιοχή Γούμερο νομού Ηλείας</t>
+  </si>
+  <si>
+    <t>κοινότητα Πάλιουρα δήμο Διρφύων Μεσσαπίων Ευβοίας</t>
+  </si>
+  <si>
+    <t>Κρήτη</t>
+  </si>
+  <si>
+    <t>Λευκίμμη Κέρκυρας</t>
+  </si>
+  <si>
+    <t>Δραπετσώνα</t>
+  </si>
+  <si>
+    <t>Καστέλλα Πειραιώς</t>
+  </si>
+  <si>
+    <t>Διεθνή Αερολιμένα Αθηνών</t>
+  </si>
+  <si>
+    <t>δήμο Κατερίνης Πιερίας</t>
+  </si>
+  <si>
+    <t>Αιγάλεω</t>
+  </si>
+  <si>
+    <t>περιοχή Ύδατα Στυγός</t>
+  </si>
+  <si>
+    <t>περιοχή Άγιος Στέφανος Αυλιωτών Κέρκυρας</t>
+  </si>
+  <si>
+    <t>οδών Χαριλάου Τρικούπη και Ναυαρίνου δήμο Αθηναίων Αττικής</t>
+  </si>
+  <si>
+    <t>περιοχή Λιχάδα Ευβοίας</t>
+  </si>
+  <si>
+    <t>δημοτική ενότητα Ιαλυσού Ρόδου</t>
+  </si>
+  <si>
+    <t>δημοτική ενότητα Πεταλούδων Ρόδου</t>
+  </si>
+  <si>
+    <t>περιοχή Μαράσια Έβρου</t>
+  </si>
+  <si>
+    <t>δασάκι Κουτσουρά δήμου Ιεράπετρας</t>
+  </si>
+  <si>
+    <t>Υπουργείο Κλιματικής Κρίσης</t>
+  </si>
+  <si>
+    <t>Αττική</t>
+  </si>
+  <si>
+    <t>περιοχή Βασιλική Λευκάδας</t>
+  </si>
+  <si>
+    <t>οδού Σεράφη δήμο Αθηναίων</t>
+  </si>
+  <si>
+    <t>Αποστόλου Παύλου Θεσσαλονίκη</t>
+  </si>
+  <si>
+    <t>οδού Σόλωνος Μενεμένη Θεσσαλονίκης</t>
+  </si>
+  <si>
+    <t>οδού Ιβήρων Αθήνα</t>
+  </si>
+  <si>
+    <t>οδού Μύρων Αθήνα</t>
+  </si>
+  <si>
+    <t>Φαράγγι Γκούρας Φυλή Αττικής</t>
+  </si>
+  <si>
+    <t>οδού Ελευθερίου Βενιζέλου Πειραιά</t>
+  </si>
+  <si>
+    <t>οδού Κωστή Παλαμά Δραπετσώνα</t>
+  </si>
+  <si>
+    <t>οδού Μ. Αλεξάνδρου δήμο Θέρμης Θεσσαλονίκης</t>
+  </si>
+  <si>
+    <t>οδών Θηβών και Πέτρου Ράλλη Αιγάλεω Αττικής</t>
+  </si>
+  <si>
+    <t>οδού Σαμαρίνας δήμο Αχαρνών Αττικής</t>
+  </si>
+  <si>
+    <t>οδού 3ης Σεπτεμβρίου Αθήνα</t>
+  </si>
+  <si>
+    <t>δημοτική κοινότητα Φύλλου δήμου Παλαμά Καρδίτσας</t>
+  </si>
+  <si>
+    <t>Λεωφόρου Δημοκρατίας Κερατσίνι Αττικής</t>
+  </si>
+  <si>
+    <t>οδού 17ης Οκτωβρίου Νάουσα Ημαθίας</t>
+  </si>
+  <si>
+    <t>οδού Εσπερίδων Κηφισιά</t>
+  </si>
+  <si>
+    <t>Λ. Συγγρού Αθήνα</t>
+  </si>
+  <si>
+    <t>οδού Αγ. Φωτεινής Ν. Σμύρνη Αττικής</t>
+  </si>
+  <si>
+    <t>περιοχή Δαύλειας Λιβαδειά Βοιωτίας</t>
+  </si>
+  <si>
+    <t>οδού Άνδρου Κορωπί</t>
+  </si>
+  <si>
+    <t>Μαρούσι Διακοπτό Αχαΐας</t>
+  </si>
+  <si>
+    <t>οδού Κυπρίων Αγωνιστών Μαρούσι Αττικής</t>
+  </si>
+  <si>
+    <t>οδού Λευκάδας Κορωπί</t>
+  </si>
+  <si>
+    <t>οδού Αναξάρχου δήμο Ξάνθης</t>
+  </si>
+  <si>
+    <t>Νέα Ποτίδαια Χαλκιδικής</t>
+  </si>
+  <si>
+    <t>περιοχή Μάραθος Ηράκλειο Κρήτης</t>
+  </si>
+  <si>
+    <t>οδού Αγρινίου δήμο Πεύκης Αττικής</t>
+  </si>
+  <si>
+    <t>οδού Ν. Παπαδημητρίου Καμένα Βούρλα Φθιωτιδας</t>
+  </si>
+  <si>
+    <t>Ε.Ο. ΑθηνώνΚορίνθου Κακιά Σκάλα Μεγάρων Σήραγγα Ευπαλίνος</t>
+  </si>
+  <si>
+    <t>Νάουσα Ημαθίας</t>
+  </si>
+  <si>
+    <t>περιοχή Καθαρό Λασιθίου</t>
+  </si>
+  <si>
+    <t>οδού Νικήτα Πειραιά</t>
+  </si>
+  <si>
+    <t>οδού Αγίου Μελετίου Αθήνα</t>
+  </si>
+  <si>
+    <t>οδού Κωννου Παλαιολόγου Νέα Ερυθραία Αττικής</t>
+  </si>
+  <si>
+    <t>οδού Μονής Πετράκη Αθήνα</t>
+  </si>
+  <si>
+    <t>Ασπρόπυργο Αττικής</t>
+  </si>
+  <si>
+    <t>οδού Ελ. Βενιζέλου Πέραμα Αττικής</t>
+  </si>
+  <si>
+    <t>Δ.Ε. Λιβαδίου Ελασσόνας Π.Ε. Λάρισας</t>
+  </si>
+  <si>
+    <t>περιοχή Πλατύ δήμου Αλεξάνδρειας Ημαθίας</t>
+  </si>
+  <si>
+    <t>Λάρισα</t>
+  </si>
+  <si>
+    <t>κόμβου Δωρικού Ε.Ο. Αλεξανδρούπολης ΒΙ.ΠΕ Αλεξανδρούπολης Έβρου</t>
+  </si>
+  <si>
+    <t>οδού Στρατάρχου Αλεξάνδρου Παπάγου Εύοσμο Θεσσαλονίκης</t>
+  </si>
+  <si>
+    <t>Πυροσβεστική Υπηρεσία Διεθνούς Αερολιμένα Αθηνών Ελευθέριος Βενιζέλος</t>
+  </si>
+  <si>
+    <t>περιοχή Χρυσοκελλαριά δήμου Πύλου Νέστορος</t>
+  </si>
+  <si>
+    <t>οδού Καλλέργη Αθήνα</t>
+  </si>
+  <si>
+    <t>Λεωφόρου Μαραθώνος Νέα Μάκρη Αττικής</t>
+  </si>
+  <si>
+    <t>οδού Ελασιδών Αθήνα</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Σε ασφαλές σημείο μεταφέρθηκε ένα σκυλάκι μετά  από πτώση του σε δύσβατο σημείο, στην περιοχή Άγιος Στέφανος Αυλιωτών Κέρκυρας. Επιχείρησαν 2 πυροσβέστες με 1 όχημα. Συνδρομή της εθελοντικής ομάδας Ε.Μ.Ε.Δ. Κέρκυρας. </t>
+  </si>
+  <si>
+    <t>περιοχή Θεοδωριανά Άρτας</t>
+  </si>
+  <si>
+    <t>οδού Πάφου δήμο Αμαρουσίου Αττικής</t>
+  </si>
+  <si>
+    <t>οδών Γαλήνης και Ρόδων Εκάλη Αττικής</t>
+  </si>
+  <si>
+    <t>οδών Συνταγματάρχου Δαβάκη και Σοφοκλέους Καλλιθέα Αττικής</t>
+  </si>
+  <si>
+    <t>επάνω Χερσόνησος δήμου Χερσονήσου Κρήτης</t>
+  </si>
+  <si>
+    <t>οδό Λιοσίων</t>
+  </si>
+  <si>
+    <t>περιοχή Θεσσαλονίκης</t>
+  </si>
+  <si>
+    <t>περιοχή Γλυφάδας</t>
+  </si>
+  <si>
+    <t>νομού Μαγνησίας</t>
+  </si>
+  <si>
+    <t>περιοχής Δήμου Αθηναίων</t>
+  </si>
+  <si>
+    <t>περιοχή Πρέβεζας</t>
+  </si>
+  <si>
+    <t>Περιφέρεια Στερεάς Ελλάδας</t>
+  </si>
+  <si>
+    <t>περιοχή Κοζάνης</t>
+  </si>
+  <si>
+    <t>περιοχής Φθιώτιδας</t>
+  </si>
+  <si>
+    <t>νομούς Καβάλας και Ξάνθης</t>
+  </si>
+  <si>
+    <t>οδό Δεκελείας Κηφισιά</t>
+  </si>
+  <si>
+    <t>Καστοριάς Γράμμου Καστοριάς</t>
+  </si>
+  <si>
+    <t>Ελλάδα</t>
+  </si>
+  <si>
+    <t>νομών Αρκαδίας και Κορινθίας</t>
+  </si>
+  <si>
+    <t>Ελληνική</t>
+  </si>
+  <si>
+    <t>Επ. οδού Σιάτοστας Κνίδης Δήμο Βοΐου Κοζάνης</t>
+  </si>
+  <si>
+    <t>Τραυματισμένος απεγκλωβίστηκε και παραδόθηκε στο ΕΚΑΒ, ένας άνδρας, συνεπεία τροχαίου, ύστερα από σύγκρουση με έτερο ΕΙΧ όχημα, επί της Επ. οδού Σιάτοστας Κνίδης στο Δήμο Βοΐου, Κοζάνης.
+Επιχείρησαν 5 πυροσβέστες με 1 όχημα.</t>
+  </si>
+  <si>
+    <t>Σορός ατόμου εντοπίστηκε κατά τη διάρκεια κατάσβεσης πυρκαγιάς σε ΕΙΧ όχημα στην Ε.Ο. Χρυσοπηγής Λακκωμάτων στο δήμο Φαρρών Αχαΐας.
+Επιχειρούν  8 πυροσβέστες με 3 οχήματα.</t>
+  </si>
+  <si>
+    <t>Ε.Ο. Χρυσοπηγής Λακκωμάτων δήμο Φαρρών Αχαΐας</t>
   </si>
 </sst>
 </file>
@@ -2482,27 +2485,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.42578125" customWidth="1"/>
     <col min="3" max="3" width="89.5703125" customWidth="1"/>
     <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -2530,10 +2533,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1.496479736087958E+18</v>
+        <v>1.4964797360879601E+18</v>
       </c>
       <c r="C3" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -2550,7 +2553,7 @@
         <v>1.496462660124226E+18</v>
       </c>
       <c r="C4" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>5</v>
@@ -2567,7 +2570,7 @@
         <v>1.496205536869728E+18</v>
       </c>
       <c r="C5" t="s">
-        <v>392</v>
+        <v>419</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -2584,7 +2587,7 @@
         <v>1.495619130669556E+18</v>
       </c>
       <c r="C6" t="s">
-        <v>393</v>
+        <v>420</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -2601,7 +2604,7 @@
         <v>1.4955983911113971E+18</v>
       </c>
       <c r="C7" t="s">
-        <v>394</v>
+        <v>421</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -2618,7 +2621,7 @@
         <v>1.4954265751727639E+18</v>
       </c>
       <c r="C8" t="s">
-        <v>395</v>
+        <v>381</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -2635,7 +2638,7 @@
         <v>1.493064014221431E+18</v>
       </c>
       <c r="C9" t="s">
-        <v>396</v>
+        <v>422</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -2652,7 +2655,7 @@
         <v>1.4947228273118001E+18</v>
       </c>
       <c r="C10" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -2669,7 +2672,7 @@
         <v>1.4946563831443661E+18</v>
       </c>
       <c r="C11" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -2686,7 +2689,7 @@
         <v>1.494552860612256E+18</v>
       </c>
       <c r="C12" t="s">
-        <v>460</v>
+        <v>385</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -2703,7 +2706,7 @@
         <v>1.49431213538766E+18</v>
       </c>
       <c r="C13" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
@@ -2720,7 +2723,7 @@
         <v>1.494038005891445E+18</v>
       </c>
       <c r="C14" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -2779,7 +2782,7 @@
         <v>1.4927544793678269E+18</v>
       </c>
       <c r="C18" t="s">
-        <v>462</v>
+        <v>401</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>19</v>
@@ -2796,7 +2799,7 @@
         <v>1.4926786114758661E+18</v>
       </c>
       <c r="C19" t="s">
-        <v>400</v>
+        <v>423</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
@@ -2813,7 +2816,7 @@
         <v>1.4921848652190021E+18</v>
       </c>
       <c r="C20" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
@@ -2830,7 +2833,7 @@
         <v>1.492132092154626E+18</v>
       </c>
       <c r="C21" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D21" t="s">
         <v>22</v>
@@ -2847,7 +2850,7 @@
         <v>1.492113436976767E+18</v>
       </c>
       <c r="C22" t="s">
-        <v>403</v>
+        <v>424</v>
       </c>
       <c r="D22" t="s">
         <v>23</v>
@@ -2864,7 +2867,7 @@
         <v>1.4920709015417411E+18</v>
       </c>
       <c r="C23" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D23" t="s">
         <v>24</v>
@@ -2881,7 +2884,7 @@
         <v>1.4920578290704881E+18</v>
       </c>
       <c r="C24" t="s">
-        <v>461</v>
+        <v>425</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>25</v>
@@ -2898,7 +2901,7 @@
         <v>1.491436312951669E+18</v>
       </c>
       <c r="C25" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D25" t="s">
         <v>26</v>
@@ -2915,7 +2918,7 @@
         <v>1.4911970611692989E+18</v>
       </c>
       <c r="C26" t="s">
-        <v>406</v>
+        <v>426</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>27</v>
@@ -2932,7 +2935,7 @@
         <v>1.4910949816791199E+18</v>
       </c>
       <c r="C27" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>28</v>
@@ -2949,7 +2952,7 @@
         <v>1.491016054327636E+18</v>
       </c>
       <c r="C28" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D28" t="s">
         <v>29</v>
@@ -2966,7 +2969,7 @@
         <v>1.4910125643563169E+18</v>
       </c>
       <c r="C29" t="s">
-        <v>409</v>
+        <v>427</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>30</v>
@@ -2983,7 +2986,7 @@
         <v>1.4904666193987011E+18</v>
       </c>
       <c r="C30" t="s">
-        <v>464</v>
+        <v>407</v>
       </c>
       <c r="D30" t="s">
         <v>31</v>
@@ -3000,10 +3003,10 @@
         <v>1.4903946393917281E+18</v>
       </c>
       <c r="C31" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D31" t="s">
-        <v>32</v>
+        <v>465</v>
       </c>
       <c r="E31" s="2">
         <v>44598.860486111109</v>
@@ -3017,10 +3020,10 @@
         <v>1.490325110905098E+18</v>
       </c>
       <c r="C32" t="s">
-        <v>464</v>
+        <v>407</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E32" s="2">
         <v>44598.668622685182</v>
@@ -3034,10 +3037,10 @@
         <v>1.490322862565122E+18</v>
       </c>
       <c r="C33" t="s">
-        <v>464</v>
+        <v>407</v>
       </c>
       <c r="D33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33" s="2">
         <v>44598.662418981483</v>
@@ -3051,10 +3054,10 @@
         <v>1.49013549454977E+18</v>
       </c>
       <c r="C34" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E34" s="2">
         <v>44598.145381944443</v>
@@ -3068,10 +3071,10 @@
         <v>1.490121458588213E+18</v>
       </c>
       <c r="C35" t="s">
-        <v>412</v>
+        <v>428</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E35" s="2">
         <v>44598.10665509259</v>
@@ -3085,10 +3088,10 @@
         <v>1.4899548776105411E+18</v>
       </c>
       <c r="C36" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E36" s="2">
         <v>44597.646979166668</v>
@@ -3102,10 +3105,10 @@
         <v>1.433366270540386E+18</v>
       </c>
       <c r="C37" t="s">
-        <v>463</v>
+        <v>429</v>
       </c>
       <c r="D37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E37" s="2">
         <v>44441.533842592587</v>
@@ -3119,10 +3122,10 @@
         <v>1.489008039596278E+18</v>
       </c>
       <c r="C38" t="s">
-        <v>414</v>
+        <v>430</v>
       </c>
       <c r="D38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E38" s="2">
         <v>44595.034201388888</v>
@@ -3136,10 +3139,10 @@
         <v>1.4890004792124129E+18</v>
       </c>
       <c r="C39" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E39" s="2">
         <v>44595.013344907413</v>
@@ -3153,10 +3156,10 @@
         <v>1.4889945235061719E+18</v>
       </c>
       <c r="C40" t="s">
-        <v>466</v>
+        <v>412</v>
       </c>
       <c r="D40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E40" s="2">
         <v>44594.99690972222</v>
@@ -3170,10 +3173,10 @@
         <v>1.4884793944862679E+18</v>
       </c>
       <c r="C41" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E41" s="2">
         <v>44593.575416666667</v>
@@ -3187,10 +3190,10 @@
         <v>1.487915151424725E+18</v>
       </c>
       <c r="C42" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E42" s="2">
         <v>44592.01840277778</v>
@@ -3204,10 +3207,10 @@
         <v>1.4879134019973079E+18</v>
       </c>
       <c r="C43" t="s">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="D43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E43" s="2">
         <v>44592.01357638889</v>
@@ -3221,10 +3224,10 @@
         <v>1.4876847100169869E+18</v>
       </c>
       <c r="C44" t="s">
-        <v>419</v>
+        <v>432</v>
       </c>
       <c r="D44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E44" s="2">
         <v>44591.382511574076</v>
@@ -3238,10 +3241,10 @@
         <v>1.4874136059182001E+18</v>
       </c>
       <c r="C45" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E45" s="2">
         <v>44590.634409722217</v>
@@ -3255,10 +3258,10 @@
         <v>1.4869962274598871E+18</v>
       </c>
       <c r="C46" t="s">
-        <v>421</v>
+        <v>433</v>
       </c>
       <c r="D46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E46" s="2">
         <v>44589.482662037037</v>
@@ -3272,7 +3275,7 @@
         <v>1.486751635573514E+18</v>
       </c>
       <c r="D47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E47" s="2">
         <v>44588.807719907411</v>
@@ -3286,10 +3289,10 @@
         <v>1.4865907942365839E+18</v>
       </c>
       <c r="C48" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="D48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E48" s="2">
         <v>44588.363877314812</v>
@@ -3303,10 +3306,10 @@
         <v>1.486362281797632E+18</v>
       </c>
       <c r="C49" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E49" s="2">
         <v>44587.733298611107</v>
@@ -3320,10 +3323,10 @@
         <v>1.486302382766047E+18</v>
       </c>
       <c r="C50" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="D50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E50" s="2">
         <v>44587.568009259259</v>
@@ -3337,10 +3340,10 @@
         <v>1.4862169617344589E+18</v>
       </c>
       <c r="C51" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="D51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E51" s="2">
         <v>44587.332291666673</v>
@@ -3354,10 +3357,10 @@
         <v>1.486125885501673E+18</v>
       </c>
       <c r="C52" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E52" s="2">
         <v>44587.080972222233</v>
@@ -3371,10 +3374,10 @@
         <v>1.47200486262385E+18</v>
       </c>
       <c r="C53" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="D53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E53" s="2">
         <v>44548.114374999997</v>
@@ -3388,10 +3391,10 @@
         <v>1.4858464273393091E+18</v>
       </c>
       <c r="C54" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="D54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E54" s="2">
         <v>44586.309814814813</v>
@@ -3405,7 +3408,7 @@
         <v>1.4857284117546391E+18</v>
       </c>
       <c r="D55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E55" s="2">
         <v>44585.984155092592</v>
@@ -3419,10 +3422,10 @@
         <v>1.4857203264284101E+18</v>
       </c>
       <c r="C56" t="s">
-        <v>426</v>
+        <v>436</v>
       </c>
       <c r="D56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E56" s="2">
         <v>44585.961840277778</v>
@@ -3436,10 +3439,10 @@
         <v>1.4855368766185229E+18</v>
       </c>
       <c r="C57" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
       <c r="D57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E57" s="2">
         <v>44585.455613425933</v>
@@ -3453,7 +3456,7 @@
         <v>1.5677588302844641E+18</v>
       </c>
       <c r="D58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E58" s="2">
         <v>44812.386655092603</v>
@@ -3467,10 +3470,10 @@
         <v>1.484506180097655E+18</v>
       </c>
       <c r="C59" t="s">
-        <v>428</v>
+        <v>438</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E59" s="2">
         <v>44582.611435185187</v>
@@ -3484,10 +3487,10 @@
         <v>1.484430676657164E+18</v>
       </c>
       <c r="C60" t="s">
-        <v>429</v>
+        <v>439</v>
       </c>
       <c r="D60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E60" s="2">
         <v>44582.403090277781</v>
@@ -3501,10 +3504,10 @@
         <v>1.4835632394222799E+18</v>
       </c>
       <c r="C61" t="s">
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="D61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E61" s="2">
         <v>44580.009421296287</v>
@@ -3518,10 +3521,10 @@
         <v>1.4834345118536699E+18</v>
       </c>
       <c r="C62" t="s">
-        <v>431</v>
+        <v>441</v>
       </c>
       <c r="D62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E62" s="2">
         <v>44579.65420138889</v>
@@ -3535,7 +3538,7 @@
         <v>1.483115891336352E+18</v>
       </c>
       <c r="D63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E63" s="2">
         <v>44578.774976851862</v>
@@ -3549,10 +3552,10 @@
         <v>1.483088644411998E+18</v>
       </c>
       <c r="C64" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="D64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E64" s="2">
         <v>44578.699780092589</v>
@@ -3566,10 +3569,10 @@
         <v>1.482814735238242E+18</v>
       </c>
       <c r="C65" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
       <c r="D65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E65" s="2">
         <v>44577.943935185183</v>
@@ -3583,10 +3586,10 @@
         <v>1.4825248905698801E+18</v>
       </c>
       <c r="C66" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="D66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E66" s="2">
         <v>44577.144120370373</v>
@@ -3600,10 +3603,10 @@
         <v>1.4825234506484979E+18</v>
       </c>
       <c r="C67" t="s">
-        <v>435</v>
+        <v>467</v>
       </c>
       <c r="D67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E67" s="2">
         <v>44577.140150462961</v>
@@ -3617,10 +3620,10 @@
         <v>1.4825125147055099E+18</v>
       </c>
       <c r="C68" t="s">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="D68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E68" s="2">
         <v>44577.109965277778</v>
@@ -3634,10 +3637,10 @@
         <v>1.482454181701108E+18</v>
       </c>
       <c r="C69" t="s">
-        <v>436</v>
+        <v>446</v>
       </c>
       <c r="D69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E69" s="2">
         <v>44576.949004629627</v>
@@ -3651,10 +3654,10 @@
         <v>1.482425824649396E+18</v>
       </c>
       <c r="C70" t="s">
-        <v>465</v>
+        <v>447</v>
       </c>
       <c r="D70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E70" s="2">
         <v>44576.870752314811</v>
@@ -3668,10 +3671,10 @@
         <v>1.4819311112950661E+18</v>
       </c>
       <c r="C71" t="s">
-        <v>437</v>
+        <v>448</v>
       </c>
       <c r="D71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E71" s="2">
         <v>44575.505601851852</v>
@@ -3685,10 +3688,10 @@
         <v>1.481865846884651E+18</v>
       </c>
       <c r="C72" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="D72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E72" s="2">
         <v>44575.325509259259</v>
@@ -3702,10 +3705,10 @@
         <v>1.448482938979594E+18</v>
       </c>
       <c r="C73" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="D73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E73" s="2">
         <v>44483.247893518521</v>
@@ -3719,10 +3722,10 @@
         <v>1.481845556083372E+18</v>
       </c>
       <c r="C74" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="D74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E74" s="2">
         <v>44575.269513888888</v>
@@ -3736,10 +3739,10 @@
         <v>1.4814368369165151E+18</v>
       </c>
       <c r="C75" t="s">
-        <v>440</v>
+        <v>451</v>
       </c>
       <c r="D75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E75" s="2">
         <v>44574.14166666667</v>
@@ -3753,10 +3756,10 @@
         <v>1.4814352425734799E+18</v>
       </c>
       <c r="C76" t="s">
-        <v>441</v>
+        <v>452</v>
       </c>
       <c r="D76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E76" s="2">
         <v>44574.13726851852</v>
@@ -3770,16 +3773,16 @@
         <v>1.4813921562585779E+18</v>
       </c>
       <c r="C77" t="s">
-        <v>442</v>
+        <v>453</v>
       </c>
       <c r="D77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E77" s="2">
         <v>44574.018368055556</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3787,10 +3790,10 @@
         <v>1.4813882358174641E+18</v>
       </c>
       <c r="C78" t="s">
-        <v>468</v>
-      </c>
-      <c r="D78" t="s">
-        <v>79</v>
+        <v>486</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>487</v>
       </c>
       <c r="E78" s="2">
         <v>44574.0075462963</v>
@@ -3804,10 +3807,10 @@
         <v>1.480362152947028E+18</v>
       </c>
       <c r="C79" t="s">
-        <v>443</v>
+        <v>469</v>
       </c>
       <c r="D79" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E79" s="2">
         <v>44571.176099537042</v>
@@ -3821,10 +3824,10 @@
         <v>1.4803204688130619E+18</v>
       </c>
       <c r="C80" t="s">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="D80" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E80" s="2">
         <v>44571.061076388891</v>
@@ -3838,10 +3841,10 @@
         <v>1.480310495781474E+18</v>
       </c>
       <c r="C81" t="s">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="D81" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E81" s="2">
         <v>44571.033553240741</v>
@@ -3855,10 +3858,10 @@
         <v>1.4801211623740291E+18</v>
       </c>
       <c r="C82" t="s">
-        <v>364</v>
+        <v>455</v>
       </c>
       <c r="D82" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E82" s="2">
         <v>44570.511099537027</v>
@@ -3872,10 +3875,10 @@
         <v>1.479258790407115E+18</v>
       </c>
       <c r="C83" t="s">
-        <v>445</v>
+        <v>456</v>
       </c>
       <c r="D83" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E83" s="2">
         <v>44568.13140046296</v>
@@ -3889,16 +3892,16 @@
         <v>1.479118702964396E+18</v>
       </c>
       <c r="C84" t="s">
-        <v>446</v>
+        <v>457</v>
       </c>
       <c r="D84" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E84" s="2">
         <v>44567.744837962957</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3906,10 +3909,10 @@
         <v>1.479035678797279E+18</v>
       </c>
       <c r="C85" t="s">
-        <v>469</v>
-      </c>
-      <c r="D85" t="s">
-        <v>86</v>
+        <v>489</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>488</v>
       </c>
       <c r="E85" s="2">
         <v>44567.515729166669</v>
@@ -3923,7 +3926,7 @@
         <v>1.4787518093847219E+18</v>
       </c>
       <c r="D86" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E86" s="2">
         <v>44566.732395833344</v>
@@ -3937,7 +3940,7 @@
         <v>1.477658075737866E+18</v>
       </c>
       <c r="D87" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E87" s="2">
         <v>44563.714270833327</v>
@@ -3951,10 +3954,10 @@
         <v>1.47708230602845E+18</v>
       </c>
       <c r="C88" t="s">
-        <v>447</v>
+        <v>468</v>
       </c>
       <c r="D88" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E88" s="2">
         <v>44562.125451388893</v>
@@ -3968,7 +3971,7 @@
         <v>1.4770379770209121E+18</v>
       </c>
       <c r="D89" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E89" s="2">
         <v>44562.003125000003</v>
@@ -3982,7 +3985,7 @@
         <v>1.4770379754185851E+18</v>
       </c>
       <c r="D90" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E90" s="2">
         <v>44562.003125000003</v>
@@ -3996,7 +3999,7 @@
         <v>1.454360607726178E+18</v>
       </c>
       <c r="D91" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E91" s="2">
         <v>44499.467175925929</v>
@@ -4010,10 +4013,10 @@
         <v>1.476950490072162E+18</v>
       </c>
       <c r="C92" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D92" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E92" s="2">
         <v>44561.761701388888</v>
@@ -4027,10 +4030,10 @@
         <v>1.4769410577409679E+18</v>
       </c>
       <c r="C93" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>448</v>
+        <v>382</v>
       </c>
       <c r="E93" s="2">
         <v>44561.735682870371</v>
@@ -4044,10 +4047,10 @@
         <v>1.4769342083586911E+18</v>
       </c>
       <c r="C94" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E94" s="2">
         <v>44561.716782407413</v>
@@ -4061,10 +4064,10 @@
         <v>1.4758449438853161E+18</v>
       </c>
       <c r="C95" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>452</v>
+        <v>383</v>
       </c>
       <c r="E95" s="2">
         <v>44558.7109837963</v>
@@ -4078,10 +4081,10 @@
         <v>1.475129417219424E+18</v>
       </c>
       <c r="C96" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="D96" t="s">
-        <v>453</v>
+        <v>384</v>
       </c>
       <c r="E96" s="2">
         <v>44556.736504629633</v>
@@ -4095,10 +4098,10 @@
         <v>1.4750229633008351E+18</v>
       </c>
       <c r="C97" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="D97" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E97" s="2">
         <v>44556.442743055559</v>
@@ -4112,10 +4115,10 @@
         <v>1.4749380474017961E+18</v>
       </c>
       <c r="C98" t="s">
-        <v>456</v>
+        <v>470</v>
       </c>
       <c r="D98" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E98" s="2">
         <v>44556.208425925928</v>
@@ -4129,10 +4132,10 @@
         <v>1.474901587831177E+18</v>
       </c>
       <c r="C99" t="s">
-        <v>457</v>
+        <v>463</v>
       </c>
       <c r="D99" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E99" s="2">
         <v>44556.107812499999</v>
@@ -4146,10 +4149,10 @@
         <v>1.473726412473442E+18</v>
       </c>
       <c r="C100" t="s">
-        <v>458</v>
+        <v>464</v>
       </c>
       <c r="D100" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E100" s="2">
         <v>44552.864942129629</v>
@@ -4163,10 +4166,10 @@
         <v>1.473701054512521E+18</v>
       </c>
       <c r="C101" t="s">
-        <v>459</v>
+        <v>435</v>
       </c>
       <c r="D101" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E101" s="2">
         <v>44552.794976851852</v>
@@ -4197,7 +4200,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -4217,7 +4220,7 @@
         <v>1.496497589189022E+18</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2">
         <v>44615.701423611114</v>
@@ -4231,7 +4234,7 @@
         <v>1.496479736087958E+18</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D3" s="2">
         <v>44615.65215277778</v>
@@ -4245,7 +4248,7 @@
         <v>1.496462660124226E+18</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D4" s="2">
         <v>44615.605034722219</v>
@@ -4259,7 +4262,7 @@
         <v>1.496205536869728E+18</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2">
         <v>44614.895509259259</v>
@@ -4273,7 +4276,7 @@
         <v>1.495619130669556E+18</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D6" s="2">
         <v>44613.277337962973</v>
@@ -4287,7 +4290,7 @@
         <v>1.4955983911113971E+18</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D7" s="2">
         <v>44613.220104166663</v>
@@ -4301,7 +4304,7 @@
         <v>1.4954265751727639E+18</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D8" s="2">
         <v>44612.745983796303</v>
@@ -4315,7 +4318,7 @@
         <v>1.493064014221431E+18</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D9" s="2">
         <v>44606.2265625</v>
@@ -4329,7 +4332,7 @@
         <v>1.4947228273118001E+18</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D10" s="2">
         <v>44610.804016203707</v>
@@ -4343,7 +4346,7 @@
         <v>1.4946563831443661E+18</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D11" s="2">
         <v>44610.620659722219</v>
@@ -4357,7 +4360,7 @@
         <v>1.494552860612256E+18</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D12" s="2">
         <v>44610.334999999999</v>
@@ -4371,7 +4374,7 @@
         <v>1.49431213538766E+18</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D13" s="2">
         <v>44609.670717592591</v>
@@ -4385,7 +4388,7 @@
         <v>1.494038005891445E+18</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D14" s="2">
         <v>44608.914270833331</v>
@@ -4399,7 +4402,7 @@
         <v>1.493679944546857E+18</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D15" s="2">
         <v>44607.926203703697</v>
@@ -4413,7 +4416,7 @@
         <v>1.4933134163999329E+18</v>
       </c>
       <c r="C16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D16" s="2">
         <v>44606.914780092593</v>
@@ -4427,7 +4430,7 @@
         <v>1.4932092611402921E+18</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D17" s="2">
         <v>44606.62736111111</v>
@@ -4441,7 +4444,7 @@
         <v>1.4927544793678269E+18</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D18" s="2">
         <v>44605.372407407413</v>
@@ -4469,7 +4472,7 @@
         <v>1.4921848652190021E+18</v>
       </c>
       <c r="C20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D20" s="2">
         <v>44603.800567129627</v>
@@ -4483,7 +4486,7 @@
         <v>1.492132092154626E+18</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D21" s="2">
         <v>44603.654942129629</v>
@@ -4497,7 +4500,7 @@
         <v>1.492113436976767E+18</v>
       </c>
       <c r="C22" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D22" s="2">
         <v>44603.603472222218</v>
@@ -4511,7 +4514,7 @@
         <v>1.4920709015417411E+18</v>
       </c>
       <c r="C23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D23" s="2">
         <v>44603.486087962963</v>
@@ -4525,7 +4528,7 @@
         <v>1.4920578290704881E+18</v>
       </c>
       <c r="C24" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D24" s="2">
         <v>44603.450023148151</v>
@@ -4539,7 +4542,7 @@
         <v>1.491436312951669E+18</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D25" s="2">
         <v>44601.734965277778</v>
@@ -4553,7 +4556,7 @@
         <v>1.4911970611692989E+18</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D26" s="2">
         <v>44601.074756944443</v>
@@ -4567,7 +4570,7 @@
         <v>1.4910949816791199E+18</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D27" s="2">
         <v>44600.793067129627</v>
@@ -4581,7 +4584,7 @@
         <v>1.491016054327636E+18</v>
       </c>
       <c r="C28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D28" s="2">
         <v>44600.575266203698</v>
@@ -4595,7 +4598,7 @@
         <v>1.4910125643563169E+18</v>
       </c>
       <c r="C29" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D29" s="2">
         <v>44600.565636574072</v>
@@ -4609,7 +4612,7 @@
         <v>1.4904666193987011E+18</v>
       </c>
       <c r="C30" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D30" s="2">
         <v>44599.059120370373</v>
@@ -4623,7 +4626,7 @@
         <v>1.4903946393917281E+18</v>
       </c>
       <c r="C31" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D31" s="2">
         <v>44598.860486111109</v>
@@ -4637,7 +4640,7 @@
         <v>1.490325110905098E+18</v>
       </c>
       <c r="C32" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D32" s="2">
         <v>44598.668622685182</v>
@@ -4651,7 +4654,7 @@
         <v>1.490322862565122E+18</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D33" s="2">
         <v>44598.662418981483</v>
@@ -4665,7 +4668,7 @@
         <v>1.49013549454977E+18</v>
       </c>
       <c r="C34" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D34" s="2">
         <v>44598.145381944443</v>
@@ -4679,7 +4682,7 @@
         <v>1.490121458588213E+18</v>
       </c>
       <c r="C35" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D35" s="2">
         <v>44598.10665509259</v>
@@ -4693,7 +4696,7 @@
         <v>1.4899548776105411E+18</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D36" s="2">
         <v>44597.646979166668</v>
@@ -4707,7 +4710,7 @@
         <v>1.433366270540386E+18</v>
       </c>
       <c r="C37" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D37" s="2">
         <v>44441.533842592587</v>
@@ -4721,7 +4724,7 @@
         <v>1.489008039596278E+18</v>
       </c>
       <c r="C38" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D38" s="2">
         <v>44595.034201388888</v>
@@ -4735,7 +4738,7 @@
         <v>1.4890004792124129E+18</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D39" s="2">
         <v>44595.013344907413</v>
@@ -4749,7 +4752,7 @@
         <v>1.4889945235061719E+18</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D40" s="2">
         <v>44594.99690972222</v>
@@ -4763,7 +4766,7 @@
         <v>1.4884793944862679E+18</v>
       </c>
       <c r="C41" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D41" s="2">
         <v>44593.575416666667</v>
@@ -4777,7 +4780,7 @@
         <v>1.487915151424725E+18</v>
       </c>
       <c r="C42" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D42" s="2">
         <v>44592.01840277778</v>
@@ -4791,7 +4794,7 @@
         <v>1.4879134019973079E+18</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D43" s="2">
         <v>44592.01357638889</v>
@@ -4805,7 +4808,7 @@
         <v>1.4876847100169869E+18</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D44" s="2">
         <v>44591.382511574076</v>
@@ -4819,7 +4822,7 @@
         <v>1.4874136059182001E+18</v>
       </c>
       <c r="C45" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D45" s="2">
         <v>44590.634409722217</v>
@@ -4833,7 +4836,7 @@
         <v>1.4869962274598871E+18</v>
       </c>
       <c r="C46" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D46" s="2">
         <v>44589.482662037037</v>
@@ -4847,7 +4850,7 @@
         <v>1.486751635573514E+18</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D47" s="2">
         <v>44588.807719907411</v>
@@ -4861,7 +4864,7 @@
         <v>1.4865907942365839E+18</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D48" s="2">
         <v>44588.363877314812</v>
@@ -4875,7 +4878,7 @@
         <v>1.486362281797632E+18</v>
       </c>
       <c r="C49" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D49" s="2">
         <v>44587.733298611107</v>
@@ -4889,7 +4892,7 @@
         <v>1.486302382766047E+18</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D50" s="2">
         <v>44587.568009259259</v>
@@ -4903,7 +4906,7 @@
         <v>1.4862169617344589E+18</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D51" s="2">
         <v>44587.332291666673</v>
@@ -4917,7 +4920,7 @@
         <v>1.486125885501673E+18</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D52" s="2">
         <v>44587.080972222233</v>
@@ -4931,7 +4934,7 @@
         <v>1.47200486262385E+18</v>
       </c>
       <c r="C53" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D53" s="2">
         <v>44548.114374999997</v>
@@ -4945,7 +4948,7 @@
         <v>1.4858464273393091E+18</v>
       </c>
       <c r="C54" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D54" s="2">
         <v>44586.309814814813</v>
@@ -4959,7 +4962,7 @@
         <v>1.4857284117546391E+18</v>
       </c>
       <c r="C55" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D55" s="2">
         <v>44585.984155092592</v>
@@ -4973,7 +4976,7 @@
         <v>1.4857203264284101E+18</v>
       </c>
       <c r="C56" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D56" s="2">
         <v>44585.961840277778</v>
@@ -4987,7 +4990,7 @@
         <v>1.4855368766185229E+18</v>
       </c>
       <c r="C57" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D57" s="2">
         <v>44585.455613425933</v>
@@ -5001,7 +5004,7 @@
         <v>1.5677588302844641E+18</v>
       </c>
       <c r="C58" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D58" s="2">
         <v>44812.386655092603</v>
@@ -5015,7 +5018,7 @@
         <v>1.484506180097655E+18</v>
       </c>
       <c r="C59" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D59" s="2">
         <v>44582.611435185187</v>
@@ -5029,7 +5032,7 @@
         <v>1.484430676657164E+18</v>
       </c>
       <c r="C60" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D60" s="2">
         <v>44582.403090277781</v>
@@ -5043,7 +5046,7 @@
         <v>1.4835632394222799E+18</v>
       </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D61" s="2">
         <v>44580.009421296287</v>
@@ -5057,7 +5060,7 @@
         <v>1.4834345118536699E+18</v>
       </c>
       <c r="C62" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D62" s="2">
         <v>44579.65420138889</v>
@@ -5071,7 +5074,7 @@
         <v>1.483115891336352E+18</v>
       </c>
       <c r="C63" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D63" s="2">
         <v>44578.774976851862</v>
@@ -5085,7 +5088,7 @@
         <v>1.483088644411998E+18</v>
       </c>
       <c r="C64" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D64" s="2">
         <v>44578.699780092589</v>
@@ -5099,7 +5102,7 @@
         <v>1.482814735238242E+18</v>
       </c>
       <c r="C65" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D65" s="2">
         <v>44577.943935185183</v>
@@ -5113,7 +5116,7 @@
         <v>1.4825248905698801E+18</v>
       </c>
       <c r="C66" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D66" s="2">
         <v>44577.144120370373</v>
@@ -5127,7 +5130,7 @@
         <v>1.4825234506484979E+18</v>
       </c>
       <c r="C67" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D67" s="2">
         <v>44577.140150462961</v>
@@ -5141,7 +5144,7 @@
         <v>1.4825125147055099E+18</v>
       </c>
       <c r="C68" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D68" s="2">
         <v>44577.109965277778</v>
@@ -5155,7 +5158,7 @@
         <v>1.482454181701108E+18</v>
       </c>
       <c r="C69" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D69" s="2">
         <v>44576.949004629627</v>
@@ -5169,7 +5172,7 @@
         <v>1.482425824649396E+18</v>
       </c>
       <c r="C70" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D70" s="2">
         <v>44576.870752314811</v>
@@ -5183,7 +5186,7 @@
         <v>1.4819311112950661E+18</v>
       </c>
       <c r="C71" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D71" s="2">
         <v>44575.505601851852</v>
@@ -5197,7 +5200,7 @@
         <v>1.481865846884651E+18</v>
       </c>
       <c r="C72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D72" s="2">
         <v>44575.325509259259</v>
@@ -5211,7 +5214,7 @@
         <v>1.448482938979594E+18</v>
       </c>
       <c r="C73" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D73" s="2">
         <v>44483.247893518521</v>
@@ -5225,7 +5228,7 @@
         <v>1.481845556083372E+18</v>
       </c>
       <c r="C74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D74" s="2">
         <v>44575.269513888888</v>
@@ -5239,7 +5242,7 @@
         <v>1.4814368369165151E+18</v>
       </c>
       <c r="C75" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D75" s="2">
         <v>44574.14166666667</v>
@@ -5253,7 +5256,7 @@
         <v>1.4814352425734799E+18</v>
       </c>
       <c r="C76" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D76" s="2">
         <v>44574.13726851852</v>
@@ -5267,7 +5270,7 @@
         <v>1.4813921562585779E+18</v>
       </c>
       <c r="C77" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D77" s="2">
         <v>44574.018368055556</v>
@@ -5281,7 +5284,7 @@
         <v>1.4813882358174641E+18</v>
       </c>
       <c r="C78" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D78" s="2">
         <v>44574.0075462963</v>
@@ -5295,7 +5298,7 @@
         <v>1.480362152947028E+18</v>
       </c>
       <c r="C79" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D79" s="2">
         <v>44571.176099537042</v>
@@ -5309,7 +5312,7 @@
         <v>1.4803204688130619E+18</v>
       </c>
       <c r="C80" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D80" s="2">
         <v>44571.061076388891</v>
@@ -5323,7 +5326,7 @@
         <v>1.480310495781474E+18</v>
       </c>
       <c r="C81" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D81" s="2">
         <v>44571.033553240741</v>
@@ -5337,7 +5340,7 @@
         <v>1.4801211623740291E+18</v>
       </c>
       <c r="C82" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D82" s="2">
         <v>44570.511099537027</v>
@@ -5351,7 +5354,7 @@
         <v>1.479258790407115E+18</v>
       </c>
       <c r="C83" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D83" s="2">
         <v>44568.13140046296</v>
@@ -5365,7 +5368,7 @@
         <v>1.479118702964396E+18</v>
       </c>
       <c r="C84" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D84" s="2">
         <v>44567.744837962957</v>
@@ -5379,7 +5382,7 @@
         <v>1.479035678797279E+18</v>
       </c>
       <c r="C85" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D85" s="2">
         <v>44567.515729166669</v>
@@ -5393,7 +5396,7 @@
         <v>1.4787518093847219E+18</v>
       </c>
       <c r="C86" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D86" s="2">
         <v>44566.732395833344</v>
@@ -5407,7 +5410,7 @@
         <v>1.477658075737866E+18</v>
       </c>
       <c r="C87" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D87" s="2">
         <v>44563.714270833327</v>
@@ -5421,7 +5424,7 @@
         <v>1.47708230602845E+18</v>
       </c>
       <c r="C88" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D88" s="2">
         <v>44562.125451388893</v>
@@ -5435,7 +5438,7 @@
         <v>1.4770379770209121E+18</v>
       </c>
       <c r="C89" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D89" s="2">
         <v>44562.003125000003</v>
@@ -5449,7 +5452,7 @@
         <v>1.4770379754185851E+18</v>
       </c>
       <c r="C90" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D90" s="2">
         <v>44562.003125000003</v>
@@ -5463,7 +5466,7 @@
         <v>1.454360607726178E+18</v>
       </c>
       <c r="C91" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D91" s="2">
         <v>44499.467175925929</v>
@@ -5477,7 +5480,7 @@
         <v>1.476950490072162E+18</v>
       </c>
       <c r="C92" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D92" s="2">
         <v>44561.761701388888</v>
@@ -5491,7 +5494,7 @@
         <v>1.4769410577409679E+18</v>
       </c>
       <c r="C93" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D93" s="2">
         <v>44561.735682870371</v>
@@ -5505,7 +5508,7 @@
         <v>1.4769342083586911E+18</v>
       </c>
       <c r="C94" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D94" s="2">
         <v>44561.716782407413</v>
@@ -5519,7 +5522,7 @@
         <v>1.4758449438853161E+18</v>
       </c>
       <c r="C95" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D95" s="2">
         <v>44558.7109837963</v>
@@ -5533,7 +5536,7 @@
         <v>1.475129417219424E+18</v>
       </c>
       <c r="C96" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D96" s="2">
         <v>44556.736504629633</v>
@@ -5547,7 +5550,7 @@
         <v>1.4750229633008351E+18</v>
       </c>
       <c r="C97" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D97" s="2">
         <v>44556.442743055559</v>
@@ -5561,7 +5564,7 @@
         <v>1.4749380474017961E+18</v>
       </c>
       <c r="C98" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D98" s="2">
         <v>44556.208425925928</v>
@@ -5575,7 +5578,7 @@
         <v>1.474901587831177E+18</v>
       </c>
       <c r="C99" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D99" s="2">
         <v>44556.107812499999</v>
@@ -5589,7 +5592,7 @@
         <v>1.473726412473442E+18</v>
       </c>
       <c r="C100" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D100" s="2">
         <v>44552.864942129629</v>
@@ -5603,7 +5606,7 @@
         <v>1.473701054512521E+18</v>
       </c>
       <c r="C101" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D101" s="2">
         <v>44552.794976851852</v>
@@ -5621,12 +5624,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="51.5703125" customWidth="1"/>
     <col min="3" max="3" width="58.85546875" customWidth="1"/>
     <col min="4" max="4" width="254.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
@@ -5634,13 +5638,13 @@
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -5657,10 +5661,10 @@
         <v>1.2593701393943759E+18</v>
       </c>
       <c r="C2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E2" s="2">
         <v>43961.395983796298</v>
@@ -5674,10 +5678,10 @@
         <v>1.262042767242519E+18</v>
       </c>
       <c r="C3" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="D3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E3" s="2">
         <v>43968.77103009259</v>
@@ -5691,10 +5695,10 @@
         <v>1.2696541320356539E+18</v>
       </c>
       <c r="C4" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E4" s="2">
         <v>43989.774398148147</v>
@@ -5708,7 +5712,7 @@
         <v>1.2731169314748211E+18</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E5" s="2">
         <v>43999.329907407409</v>
@@ -5722,10 +5726,10 @@
         <v>1.2736061508193651E+18</v>
       </c>
       <c r="C6" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="D6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E6" s="2">
         <v>44000.679895833331</v>
@@ -5739,10 +5743,10 @@
         <v>1.2760779235570481E+18</v>
       </c>
       <c r="C7" t="s">
-        <v>472</v>
+        <v>386</v>
       </c>
       <c r="D7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E7" s="2">
         <v>44007.500694444447</v>
@@ -5756,7 +5760,7 @@
         <v>1.2763784237247731E+18</v>
       </c>
       <c r="D8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E8" s="2">
         <v>44008.329907407409</v>
@@ -5770,10 +5774,10 @@
         <v>1.2590681600550909E+18</v>
       </c>
       <c r="C9" t="s">
-        <v>368</v>
+        <v>482</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E9" s="2">
         <v>43960.562685185178</v>
@@ -5787,7 +5791,7 @@
         <v>1.278551491108844E+18</v>
       </c>
       <c r="D10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E10" s="2">
         <v>44014.326435185183</v>
@@ -5801,7 +5805,7 @@
         <v>1.2789138768857541E+18</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E11" s="2">
         <v>44015.326423611114</v>
@@ -5815,7 +5819,7 @@
         <v>1.2814506001196521E+18</v>
       </c>
       <c r="D12" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E12" s="2">
         <v>44022.32644675926</v>
@@ -5829,7 +5833,7 @@
         <v>1.282900142035735E+18</v>
       </c>
       <c r="D13" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E13" s="2">
         <v>44026.326423611114</v>
@@ -5843,7 +5847,7 @@
         <v>1.2836249157789E+18</v>
       </c>
       <c r="D14" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E14" s="2">
         <v>44028.326423611114</v>
@@ -5857,10 +5861,10 @@
         <v>1.2865643788301481E+18</v>
       </c>
       <c r="C15" t="s">
-        <v>473</v>
+        <v>387</v>
       </c>
       <c r="D15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E15" s="2">
         <v>44036.437789351847</v>
@@ -5873,8 +5877,11 @@
       <c r="B16">
         <v>1.2891639366804851E+18</v>
       </c>
+      <c r="C16" t="s">
+        <v>483</v>
+      </c>
       <c r="D16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E16" s="2">
         <v>44043.611203703702</v>
@@ -5888,7 +5895,7 @@
         <v>1.292680835867595E+18</v>
       </c>
       <c r="D17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E17" s="2">
         <v>44053.315995370373</v>
@@ -5902,10 +5909,10 @@
         <v>1.29465133464653E+18</v>
       </c>
       <c r="C18" t="s">
-        <v>473</v>
+        <v>387</v>
       </c>
       <c r="D18" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E18" s="2">
         <v>44058.753541666672</v>
@@ -5919,10 +5926,10 @@
         <v>1.2591184502340851E+18</v>
       </c>
       <c r="C19" t="s">
-        <v>369</v>
+        <v>484</v>
       </c>
       <c r="D19" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E19" s="2">
         <v>43960.701458333337</v>
@@ -5936,10 +5943,10 @@
         <v>1.3090348511363479E+18</v>
       </c>
       <c r="C20" t="s">
-        <v>474</v>
+        <v>388</v>
       </c>
       <c r="D20" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E20" s="2">
         <v>44098.444479166668</v>
@@ -5953,10 +5960,10 @@
         <v>1.286931691450388E+18</v>
       </c>
       <c r="C21" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="D21" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E21" s="2">
         <v>44037.451377314806</v>
@@ -5970,7 +5977,7 @@
         <v>1.313340720321909E+18</v>
       </c>
       <c r="D22" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E22" s="2">
         <v>44110.326423611114</v>
@@ -5984,7 +5991,7 @@
         <v>1.259709604243669E+18</v>
       </c>
       <c r="D23" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E23" s="2">
         <v>43962.332731481481</v>
@@ -5998,10 +6005,10 @@
         <v>1.2822836374347039E+18</v>
       </c>
       <c r="C24" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D24" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E24" s="2">
         <v>44024.625196759262</v>
@@ -6015,10 +6022,10 @@
         <v>1.3207709396934861E+18</v>
       </c>
       <c r="C25" t="s">
-        <v>476</v>
+        <v>389</v>
       </c>
       <c r="D25" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E25" s="2">
         <v>44130.788252314807</v>
@@ -6032,7 +6039,7 @@
         <v>1.260068462858326E+18</v>
       </c>
       <c r="D26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E26" s="2">
         <v>43963.322997685187</v>
@@ -6046,10 +6053,10 @@
         <v>1.276784859235734E+18</v>
       </c>
       <c r="C27" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="D27" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E27" s="2">
         <v>44009.451458333337</v>
@@ -6063,10 +6070,10 @@
         <v>1.330415730794377E+18</v>
       </c>
       <c r="C28" t="s">
-        <v>473</v>
+        <v>387</v>
       </c>
       <c r="D28" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E28" s="2">
         <v>44157.402800925927</v>
@@ -6080,10 +6087,10 @@
         <v>1.271059316770996E+18</v>
       </c>
       <c r="C29" t="s">
-        <v>478</v>
+        <v>390</v>
       </c>
       <c r="D29" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E29" s="2">
         <v>43993.651967592603</v>
@@ -6097,10 +6104,10 @@
         <v>1.260245777441599E+18</v>
       </c>
       <c r="C30" t="s">
-        <v>479</v>
+        <v>391</v>
       </c>
       <c r="D30" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E30" s="2">
         <v>43963.812291666669</v>
@@ -6114,7 +6121,7 @@
         <v>1.2604320938609869E+18</v>
       </c>
       <c r="D31" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E31" s="2">
         <v>43964.326423611114</v>
@@ -6128,7 +6135,7 @@
         <v>1.2607944885171651E+18</v>
       </c>
       <c r="D32" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E32" s="2">
         <v>43965.32644675926</v>
@@ -6142,7 +6149,7 @@
         <v>1.266231560610562E+18</v>
       </c>
       <c r="D33" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E33" s="2">
         <v>43980.329907407409</v>
@@ -6156,10 +6163,10 @@
         <v>1.286932001342263E+18</v>
       </c>
       <c r="C34" t="s">
-        <v>480</v>
+        <v>392</v>
       </c>
       <c r="D34" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E34" s="2">
         <v>44037.452233796299</v>
@@ -6173,10 +6180,10 @@
         <v>1.3180945496344581E+18</v>
       </c>
       <c r="C35" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="D35" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E35" s="2">
         <v>44123.444490740738</v>
@@ -6190,10 +6197,10 @@
         <v>1.3301201578349811E+18</v>
       </c>
       <c r="C36" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D36" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E36" s="2">
         <v>44156.587175925917</v>
@@ -6207,10 +6214,10 @@
         <v>1.356858718651113E+18</v>
       </c>
       <c r="C37" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D37" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E37" s="2">
         <v>44230.371550925927</v>
@@ -6224,7 +6231,7 @@
         <v>1.414993192739541E+18</v>
       </c>
       <c r="D38" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E38" s="2">
         <v>44390.833807870367</v>
@@ -6238,7 +6245,7 @@
         <v>1.435233914201719E+18</v>
       </c>
       <c r="D39" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E39" s="2">
         <v>44446.687557870369</v>
@@ -6252,10 +6259,10 @@
         <v>1.4706409089997371E+18</v>
       </c>
       <c r="C40" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="D40" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E40" s="2">
         <v>44544.350578703707</v>
@@ -6269,7 +6276,7 @@
         <v>1.492820731339682E+18</v>
       </c>
       <c r="D41" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E41" s="2">
         <v>44605.555231481478</v>
@@ -6283,10 +6290,10 @@
         <v>1.262304156892778E+18</v>
       </c>
       <c r="C42" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D42" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E42" s="2">
         <v>43969.492337962962</v>
@@ -6300,10 +6307,10 @@
         <v>1.2731486275490691E+18</v>
       </c>
       <c r="C43" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="D43" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E43" s="2">
         <v>43999.417372685188</v>
@@ -6320,7 +6327,7 @@
         <v>481</v>
       </c>
       <c r="D44" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E44" s="2">
         <v>44033.429837962962</v>
@@ -6334,10 +6341,10 @@
         <v>1.286932244729344E+18</v>
       </c>
       <c r="C45" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D45" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E45" s="2">
         <v>44037.452905092592</v>
@@ -6351,7 +6358,7 @@
         <v>1.2905102865548979E+18</v>
       </c>
       <c r="D46" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E46" s="2">
         <v>44047.326423611114</v>
@@ -6365,10 +6372,10 @@
         <v>1.2964633217811991E+18</v>
       </c>
       <c r="C47" t="s">
-        <v>376</v>
+        <v>475</v>
       </c>
       <c r="D47" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E47" s="2">
         <v>44063.753668981481</v>
@@ -6382,10 +6389,10 @@
         <v>1.3117002232412119E+18</v>
       </c>
       <c r="C48" t="s">
-        <v>482</v>
+        <v>393</v>
       </c>
       <c r="D48" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E48" s="2">
         <v>44105.799513888887</v>
@@ -6399,10 +6406,10 @@
         <v>1.33981272340897E+18</v>
       </c>
       <c r="C49" t="s">
-        <v>483</v>
+        <v>394</v>
       </c>
       <c r="D49" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E49" s="2">
         <v>44183.333564814813</v>
@@ -6416,7 +6423,7 @@
         <v>1.352207800408158E+18</v>
       </c>
       <c r="D50" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E50" s="2">
         <v>44217.537465277783</v>
@@ -6430,10 +6437,10 @@
         <v>1.3199075908774459E+18</v>
       </c>
       <c r="C51" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="D51" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E51" s="2">
         <v>44128.447534722232</v>
@@ -6447,10 +6454,10 @@
         <v>1.4469058167627571E+18</v>
       </c>
       <c r="C52" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="D52" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E52" s="2">
         <v>44478.895868055559</v>
@@ -6464,10 +6471,10 @@
         <v>1.3236599861452879E+18</v>
       </c>
       <c r="C53" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="D53" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E53" s="2">
         <v>44138.760497685187</v>
@@ -6481,10 +6488,10 @@
         <v>1.477572892686975E+18</v>
       </c>
       <c r="C54" t="s">
-        <v>483</v>
+        <v>394</v>
       </c>
       <c r="D54" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="E54" s="2">
         <v>44563.479212962957</v>
@@ -6498,7 +6505,7 @@
         <v>1.491287008077132E+18</v>
       </c>
       <c r="D55" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E55" s="2">
         <v>44601.322962962957</v>
@@ -6512,7 +6519,7 @@
         <v>1.491650647984427E+18</v>
       </c>
       <c r="D56" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E56" s="2">
         <v>44602.326412037037</v>
@@ -6526,7 +6533,7 @@
         <v>1.4920130367391739E+18</v>
       </c>
       <c r="D57" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E57" s="2">
         <v>44603.326412037037</v>
@@ -6540,7 +6547,7 @@
         <v>1.4931035460442319E+18</v>
       </c>
       <c r="D58" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E58" s="2">
         <v>44606.335648148153</v>
@@ -6554,7 +6561,7 @@
         <v>1.4934625871530391E+18</v>
       </c>
       <c r="D59" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E59" s="2">
         <v>44607.326412037037</v>
@@ -6568,7 +6575,7 @@
         <v>1.493824975232406E+18</v>
       </c>
       <c r="D60" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E60" s="2">
         <v>44608.326412037037</v>
@@ -6582,7 +6589,7 @@
         <v>1.4941873601117061E+18</v>
       </c>
       <c r="D61" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E61" s="2">
         <v>44609.32640046296</v>
@@ -6596,10 +6603,10 @@
         <v>1.2601062137585129E+18</v>
       </c>
       <c r="C62" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="D62" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E62" s="2">
         <v>43963.427164351851</v>
@@ -6613,7 +6620,7 @@
         <v>1.261155615386239E+18</v>
       </c>
       <c r="D63" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E63" s="2">
         <v>43966.322962962957</v>
@@ -6627,7 +6634,7 @@
         <v>1.2622490725529679E+18</v>
       </c>
       <c r="D64" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E64" s="2">
         <v>43969.34033564815</v>
@@ -6641,10 +6648,10 @@
         <v>1.2623472233225631E+18</v>
       </c>
       <c r="C65" t="s">
-        <v>484</v>
+        <v>395</v>
       </c>
       <c r="D65" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E65" s="2">
         <v>43969.611168981479</v>
@@ -6658,10 +6665,10 @@
         <v>1.262442993371529E+18</v>
       </c>
       <c r="C66" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D66" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E66" s="2">
         <v>43969.875451388893</v>
@@ -6675,7 +6682,7 @@
         <v>1.262605165254902E+18</v>
       </c>
       <c r="D67" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E67" s="2">
         <v>43970.322962962957</v>
@@ -6689,10 +6696,10 @@
         <v>1.262646747127562E+18</v>
       </c>
       <c r="C68" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="D68" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E68" s="2">
         <v>43970.437708333331</v>
@@ -6706,10 +6713,10 @@
         <v>1.262770019949216E+18</v>
       </c>
       <c r="C69" t="s">
-        <v>485</v>
+        <v>396</v>
       </c>
       <c r="D69" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E69" s="2">
         <v>43970.777870370373</v>
@@ -6723,7 +6730,7 @@
         <v>1.2629688115585229E+18</v>
       </c>
       <c r="D70" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E70" s="2">
         <v>43971.326435185183</v>
@@ -6737,7 +6744,7 @@
         <v>1.263331198220276E+18</v>
       </c>
       <c r="D71" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E71" s="2">
         <v>43972.326423611114</v>
@@ -6751,7 +6758,7 @@
         <v>1.26369358686609E+18</v>
       </c>
       <c r="D72" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E72" s="2">
         <v>43973.326435185183</v>
@@ -6765,10 +6772,10 @@
         <v>1.2638609770927549E+18</v>
       </c>
       <c r="C73" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D73" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E73" s="2">
         <v>43973.78833333333</v>
@@ -6782,10 +6789,10 @@
         <v>1.2640811703310541E+18</v>
       </c>
       <c r="C74" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="D74" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E74" s="2">
         <v>43974.395960648151</v>
@@ -6799,7 +6806,7 @@
         <v>1.264780749774954E+18</v>
       </c>
       <c r="D75" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E75" s="2">
         <v>43976.326423611114</v>
@@ -6813,7 +6820,7 @@
         <v>1.2648499612393549E+18</v>
       </c>
       <c r="D76" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="E76" s="2">
         <v>43976.517418981479</v>
@@ -6827,7 +6834,7 @@
         <v>1.265143134406795E+18</v>
       </c>
       <c r="D77" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E77" s="2">
         <v>43977.326423611114</v>
@@ -6841,10 +6848,10 @@
         <v>1.265182159188439E+18</v>
       </c>
       <c r="C78" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="D78" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E78" s="2">
         <v>43977.434108796297</v>
@@ -6858,10 +6865,10 @@
         <v>1.3272782488128141E+18</v>
       </c>
       <c r="C79" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="D79" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E79" s="2">
         <v>44148.745000000003</v>
@@ -6875,21 +6882,21 @@
         <v>1.265505527406174E+18</v>
       </c>
       <c r="D80" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E80" s="2">
         <v>43978.326435185183</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
       <c r="B81">
         <v>1.2658691767464509E+18</v>
       </c>
-      <c r="D81" t="s">
-        <v>248</v>
+      <c r="D81" s="6" t="s">
+        <v>245</v>
       </c>
       <c r="E81" s="2">
         <v>43979.329918981479</v>
@@ -6903,7 +6910,7 @@
         <v>1.2673174636891871E+18</v>
       </c>
       <c r="D82" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E82" s="2">
         <v>43983.326423611114</v>
@@ -6917,7 +6924,7 @@
         <v>1.267679850996937E+18</v>
       </c>
       <c r="D83" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E83" s="2">
         <v>43984.326423611114</v>
@@ -6931,7 +6938,7 @@
         <v>1.2680434993809039E+18</v>
       </c>
       <c r="D84" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E84" s="2">
         <v>43985.329907407409</v>
@@ -6945,7 +6952,7 @@
         <v>1.2684058861350221E+18</v>
       </c>
       <c r="D85" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E85" s="2">
         <v>43986.329895833333</v>
@@ -6959,7 +6966,7 @@
         <v>1.268768274629759E+18</v>
       </c>
       <c r="D86" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E86" s="2">
         <v>43987.329895833333</v>
@@ -6972,8 +6979,11 @@
       <c r="B87">
         <v>1.26995235389936E+18</v>
       </c>
+      <c r="C87" t="s">
+        <v>485</v>
+      </c>
       <c r="D87" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E87" s="2">
         <v>43990.597337962958</v>
@@ -6987,7 +6997,7 @@
         <v>1.2702116048488161E+18</v>
       </c>
       <c r="D88" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E88" s="2">
         <v>43991.312731481477</v>
@@ -7001,10 +7011,10 @@
         <v>1.2703286074041549E+18</v>
       </c>
       <c r="C89" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="D89" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E89" s="2">
         <v>43991.635601851849</v>
@@ -7018,7 +7028,7 @@
         <v>1.2705751779282371E+18</v>
       </c>
       <c r="D90" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E90" s="2">
         <v>43992.316006944442</v>
@@ -7032,7 +7042,7 @@
         <v>1.2709401002565839E+18</v>
       </c>
       <c r="D91" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E91" s="2">
         <v>43993.322997685187</v>
@@ -7046,10 +7056,10 @@
         <v>1.2709701653086369E+18</v>
       </c>
       <c r="C92" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="D92" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E92" s="2">
         <v>43993.405960648153</v>
@@ -7063,10 +7073,10 @@
         <v>1.271004517421781E+18</v>
       </c>
       <c r="C93" t="s">
-        <v>386</v>
+        <v>474</v>
       </c>
       <c r="D93" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E93" s="2">
         <v>43993.500752314823</v>
@@ -7080,7 +7090,7 @@
         <v>1.2713024845317819E+18</v>
       </c>
       <c r="D94" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E94" s="2">
         <v>43994.32298611111</v>
@@ -7094,10 +7104,10 @@
         <v>1.2717745957297559E+18</v>
       </c>
       <c r="C95" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D95" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E95" s="2">
         <v>43995.625763888893</v>
@@ -7111,10 +7121,10 @@
         <v>1.2720613426194839E+18</v>
       </c>
       <c r="C96" t="s">
-        <v>487</v>
+        <v>476</v>
       </c>
       <c r="D96" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E96" s="2">
         <v>43996.417037037027</v>
@@ -7128,10 +7138,10 @@
         <v>1.2721040051965499E+18</v>
       </c>
       <c r="C97" t="s">
-        <v>387</v>
+        <v>477</v>
       </c>
       <c r="D97" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E97" s="2">
         <v>43996.534768518519</v>
@@ -7145,7 +7155,7 @@
         <v>1.2723883792048251E+18</v>
       </c>
       <c r="D98" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E98" s="2">
         <v>43997.319490740738</v>
@@ -7159,10 +7169,10 @@
         <v>1.272431292773216E+18</v>
       </c>
       <c r="C99" t="s">
-        <v>388</v>
+        <v>478</v>
       </c>
       <c r="D99" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E99" s="2">
         <v>43997.437905092593</v>
@@ -7176,7 +7186,7 @@
         <v>1.272752042709332E+18</v>
       </c>
       <c r="D100" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E100" s="2">
         <v>43998.323009259257</v>
@@ -7190,10 +7200,10 @@
         <v>1.2732573667299981E+18</v>
       </c>
       <c r="C101" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="D101" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E101" s="2">
         <v>43999.717430555553</v>
@@ -7211,8 +7221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7223,7 +7233,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -7243,7 +7253,7 @@
         <v>1.2593701393943759E+18</v>
       </c>
       <c r="C2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D2" s="2">
         <v>43961.395983796298</v>
@@ -7257,7 +7267,7 @@
         <v>1.262042767242519E+18</v>
       </c>
       <c r="C3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D3" s="2">
         <v>43968.77103009259</v>
@@ -7271,7 +7281,7 @@
         <v>1.2696541320356539E+18</v>
       </c>
       <c r="C4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D4" s="2">
         <v>43989.774398148147</v>
@@ -7285,7 +7295,7 @@
         <v>1.2731169314748211E+18</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D5" s="2">
         <v>43999.329907407409</v>
@@ -7299,7 +7309,7 @@
         <v>1.2736061508193651E+18</v>
       </c>
       <c r="C6" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D6" s="2">
         <v>44000.679895833331</v>
@@ -7313,7 +7323,7 @@
         <v>1.2760779235570481E+18</v>
       </c>
       <c r="C7" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D7" s="2">
         <v>44007.500694444447</v>
@@ -7327,7 +7337,7 @@
         <v>1.2763784237247731E+18</v>
       </c>
       <c r="C8" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D8" s="2">
         <v>44008.329907407409</v>
@@ -7341,7 +7351,7 @@
         <v>1.2590681600550909E+18</v>
       </c>
       <c r="C9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D9" s="2">
         <v>43960.562685185178</v>
@@ -7355,7 +7365,7 @@
         <v>1.278551491108844E+18</v>
       </c>
       <c r="C10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D10" s="2">
         <v>44014.326435185183</v>
@@ -7369,7 +7379,7 @@
         <v>1.2789138768857541E+18</v>
       </c>
       <c r="C11" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D11" s="2">
         <v>44015.326423611114</v>
@@ -7383,7 +7393,7 @@
         <v>1.2814506001196521E+18</v>
       </c>
       <c r="C12" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D12" s="2">
         <v>44022.32644675926</v>
@@ -7397,7 +7407,7 @@
         <v>1.282900142035735E+18</v>
       </c>
       <c r="C13" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D13" s="2">
         <v>44026.326423611114</v>
@@ -7411,7 +7421,7 @@
         <v>1.2836249157789E+18</v>
       </c>
       <c r="C14" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D14" s="2">
         <v>44028.326423611114</v>
@@ -7425,7 +7435,7 @@
         <v>1.2865643788301481E+18</v>
       </c>
       <c r="C15" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D15" s="2">
         <v>44036.437789351847</v>
@@ -7439,7 +7449,7 @@
         <v>1.2891639366804851E+18</v>
       </c>
       <c r="C16" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D16" s="2">
         <v>44043.611203703702</v>
@@ -7453,7 +7463,7 @@
         <v>1.292680835867595E+18</v>
       </c>
       <c r="C17" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D17" s="2">
         <v>44053.315995370373</v>
@@ -7467,7 +7477,7 @@
         <v>1.29465133464653E+18</v>
       </c>
       <c r="C18" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D18" s="2">
         <v>44058.753541666672</v>
@@ -7481,7 +7491,7 @@
         <v>1.2591184502340851E+18</v>
       </c>
       <c r="C19" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D19" s="2">
         <v>43960.701458333337</v>
@@ -7495,7 +7505,7 @@
         <v>1.3090348511363479E+18</v>
       </c>
       <c r="C20" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D20" s="2">
         <v>44098.444479166668</v>
@@ -7509,7 +7519,7 @@
         <v>1.286931691450388E+18</v>
       </c>
       <c r="C21" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D21" s="2">
         <v>44037.451377314806</v>
@@ -7523,7 +7533,7 @@
         <v>1.313340720321909E+18</v>
       </c>
       <c r="C22" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D22" s="2">
         <v>44110.326423611114</v>
@@ -7537,7 +7547,7 @@
         <v>1.259709604243669E+18</v>
       </c>
       <c r="C23" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D23" s="2">
         <v>43962.332731481481</v>
@@ -7551,7 +7561,7 @@
         <v>1.2822836374347039E+18</v>
       </c>
       <c r="C24" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D24" s="2">
         <v>44024.625196759262</v>
@@ -7565,7 +7575,7 @@
         <v>1.3207709396934861E+18</v>
       </c>
       <c r="C25" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D25" s="2">
         <v>44130.788252314807</v>
@@ -7579,7 +7589,7 @@
         <v>1.260068462858326E+18</v>
       </c>
       <c r="C26" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D26" s="2">
         <v>43963.322997685187</v>
@@ -7593,7 +7603,7 @@
         <v>1.276784859235734E+18</v>
       </c>
       <c r="C27" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D27" s="2">
         <v>44009.451458333337</v>
@@ -7607,7 +7617,7 @@
         <v>1.330415730794377E+18</v>
       </c>
       <c r="C28" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D28" s="2">
         <v>44157.402800925927</v>
@@ -7621,7 +7631,7 @@
         <v>1.271059316770996E+18</v>
       </c>
       <c r="C29" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D29" s="2">
         <v>43993.651967592603</v>
@@ -7635,7 +7645,7 @@
         <v>1.260245777441599E+18</v>
       </c>
       <c r="C30" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D30" s="2">
         <v>43963.812291666669</v>
@@ -7649,7 +7659,7 @@
         <v>1.2604320938609869E+18</v>
       </c>
       <c r="C31" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D31" s="2">
         <v>43964.326423611114</v>
@@ -7663,7 +7673,7 @@
         <v>1.2607944885171651E+18</v>
       </c>
       <c r="C32" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D32" s="2">
         <v>43965.32644675926</v>
@@ -7677,7 +7687,7 @@
         <v>1.266231560610562E+18</v>
       </c>
       <c r="C33" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D33" s="2">
         <v>43980.329907407409</v>
@@ -7691,7 +7701,7 @@
         <v>1.286932001342263E+18</v>
       </c>
       <c r="C34" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D34" s="2">
         <v>44037.452233796299</v>
@@ -7705,7 +7715,7 @@
         <v>1.3180945496344581E+18</v>
       </c>
       <c r="C35" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D35" s="2">
         <v>44123.444490740738</v>
@@ -7719,7 +7729,7 @@
         <v>1.3301201578349811E+18</v>
       </c>
       <c r="C36" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D36" s="2">
         <v>44156.587175925917</v>
@@ -7733,7 +7743,7 @@
         <v>1.356858718651113E+18</v>
       </c>
       <c r="C37" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D37" s="2">
         <v>44230.371550925927</v>
@@ -7747,7 +7757,7 @@
         <v>1.414993192739541E+18</v>
       </c>
       <c r="C38" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D38" s="2">
         <v>44390.833807870367</v>
@@ -7761,7 +7771,7 @@
         <v>1.435233914201719E+18</v>
       </c>
       <c r="C39" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D39" s="2">
         <v>44446.687557870369</v>
@@ -7775,7 +7785,7 @@
         <v>1.4706409089997371E+18</v>
       </c>
       <c r="C40" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D40" s="2">
         <v>44544.350578703707</v>
@@ -7789,7 +7799,7 @@
         <v>1.492820731339682E+18</v>
       </c>
       <c r="C41" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D41" s="2">
         <v>44605.555231481478</v>
@@ -7803,7 +7813,7 @@
         <v>1.262304156892778E+18</v>
       </c>
       <c r="C42" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D42" s="2">
         <v>43969.492337962962</v>
@@ -7817,7 +7827,7 @@
         <v>1.2731486275490691E+18</v>
       </c>
       <c r="C43" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D43" s="2">
         <v>43999.417372685188</v>
@@ -7831,7 +7841,7 @@
         <v>1.2854743306427231E+18</v>
       </c>
       <c r="C44" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D44" s="2">
         <v>44033.429837962962</v>
@@ -7845,7 +7855,7 @@
         <v>1.286932244729344E+18</v>
       </c>
       <c r="C45" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D45" s="2">
         <v>44037.452905092592</v>
@@ -7859,7 +7869,7 @@
         <v>1.2905102865548979E+18</v>
       </c>
       <c r="C46" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D46" s="2">
         <v>44047.326423611114</v>
@@ -7873,7 +7883,7 @@
         <v>1.2964633217811991E+18</v>
       </c>
       <c r="C47" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D47" s="2">
         <v>44063.753668981481</v>
@@ -7887,7 +7897,7 @@
         <v>1.3117002232412119E+18</v>
       </c>
       <c r="C48" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D48" s="2">
         <v>44105.799513888887</v>
@@ -7901,7 +7911,7 @@
         <v>1.33981272340897E+18</v>
       </c>
       <c r="C49" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D49" s="2">
         <v>44183.333564814813</v>
@@ -7915,7 +7925,7 @@
         <v>1.352207800408158E+18</v>
       </c>
       <c r="C50" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D50" s="2">
         <v>44217.537465277783</v>
@@ -7929,7 +7939,7 @@
         <v>1.3199075908774459E+18</v>
       </c>
       <c r="C51" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D51" s="2">
         <v>44128.447534722232</v>
@@ -7943,7 +7953,7 @@
         <v>1.4469058167627571E+18</v>
       </c>
       <c r="C52" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D52" s="2">
         <v>44478.895868055559</v>
@@ -7957,7 +7967,7 @@
         <v>1.3236599861452879E+18</v>
       </c>
       <c r="C53" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D53" s="2">
         <v>44138.760497685187</v>
@@ -7971,7 +7981,7 @@
         <v>1.477572892686975E+18</v>
       </c>
       <c r="C54" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D54" s="2">
         <v>44563.479212962957</v>
@@ -7985,7 +7995,7 @@
         <v>1.491287008077132E+18</v>
       </c>
       <c r="C55" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D55" s="2">
         <v>44601.322962962957</v>
@@ -7999,7 +8009,7 @@
         <v>1.491650647984427E+18</v>
       </c>
       <c r="C56" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D56" s="2">
         <v>44602.326412037037</v>
@@ -8013,7 +8023,7 @@
         <v>1.4920130367391739E+18</v>
       </c>
       <c r="C57" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D57" s="2">
         <v>44603.326412037037</v>
@@ -8027,7 +8037,7 @@
         <v>1.4931035460442319E+18</v>
       </c>
       <c r="C58" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D58" s="2">
         <v>44606.335648148153</v>
@@ -8041,7 +8051,7 @@
         <v>1.4934625871530391E+18</v>
       </c>
       <c r="C59" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D59" s="2">
         <v>44607.326412037037</v>
@@ -8055,7 +8065,7 @@
         <v>1.493824975232406E+18</v>
       </c>
       <c r="C60" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D60" s="2">
         <v>44608.326412037037</v>
@@ -8069,7 +8079,7 @@
         <v>1.4941873601117061E+18</v>
       </c>
       <c r="C61" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D61" s="2">
         <v>44609.32640046296</v>
@@ -8083,7 +8093,7 @@
         <v>1.2601062137585129E+18</v>
       </c>
       <c r="C62" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D62" s="2">
         <v>43963.427164351851</v>
@@ -8097,7 +8107,7 @@
         <v>1.261155615386239E+18</v>
       </c>
       <c r="C63" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D63" s="2">
         <v>43966.322962962957</v>
@@ -8111,7 +8121,7 @@
         <v>1.2622490725529679E+18</v>
       </c>
       <c r="C64" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D64" s="2">
         <v>43969.34033564815</v>
@@ -8125,7 +8135,7 @@
         <v>1.2623472233225631E+18</v>
       </c>
       <c r="C65" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D65" s="2">
         <v>43969.611168981479</v>
@@ -8139,7 +8149,7 @@
         <v>1.262442993371529E+18</v>
       </c>
       <c r="C66" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D66" s="2">
         <v>43969.875451388893</v>
@@ -8153,7 +8163,7 @@
         <v>1.262605165254902E+18</v>
       </c>
       <c r="C67" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D67" s="2">
         <v>43970.322962962957</v>
@@ -8167,7 +8177,7 @@
         <v>1.262646747127562E+18</v>
       </c>
       <c r="C68" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D68" s="2">
         <v>43970.437708333331</v>
@@ -8181,7 +8191,7 @@
         <v>1.262770019949216E+18</v>
       </c>
       <c r="C69" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D69" s="2">
         <v>43970.777870370373</v>
@@ -8195,7 +8205,7 @@
         <v>1.2629688115585229E+18</v>
       </c>
       <c r="C70" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D70" s="2">
         <v>43971.326435185183</v>
@@ -8209,7 +8219,7 @@
         <v>1.263331198220276E+18</v>
       </c>
       <c r="C71" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D71" s="2">
         <v>43972.326423611114</v>
@@ -8223,7 +8233,7 @@
         <v>1.26369358686609E+18</v>
       </c>
       <c r="C72" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D72" s="2">
         <v>43973.326435185183</v>
@@ -8237,7 +8247,7 @@
         <v>1.2638609770927549E+18</v>
       </c>
       <c r="C73" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D73" s="2">
         <v>43973.78833333333</v>
@@ -8251,7 +8261,7 @@
         <v>1.2640811703310541E+18</v>
       </c>
       <c r="C74" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D74" s="2">
         <v>43974.395960648151</v>
@@ -8265,7 +8275,7 @@
         <v>1.264780749774954E+18</v>
       </c>
       <c r="C75" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D75" s="2">
         <v>43976.326423611114</v>
@@ -8279,7 +8289,7 @@
         <v>1.2648499612393549E+18</v>
       </c>
       <c r="C76" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D76" s="2">
         <v>43976.517418981479</v>
@@ -8293,7 +8303,7 @@
         <v>1.265143134406795E+18</v>
       </c>
       <c r="C77" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D77" s="2">
         <v>43977.326423611114</v>
@@ -8307,7 +8317,7 @@
         <v>1.265182159188439E+18</v>
       </c>
       <c r="C78" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D78" s="2">
         <v>43977.434108796297</v>
@@ -8321,7 +8331,7 @@
         <v>1.3272782488128141E+18</v>
       </c>
       <c r="C79" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D79" s="2">
         <v>44148.745000000003</v>
@@ -8335,7 +8345,7 @@
         <v>1.265505527406174E+18</v>
       </c>
       <c r="C80" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D80" s="2">
         <v>43978.326435185183</v>
@@ -8349,7 +8359,7 @@
         <v>1.2658691767464509E+18</v>
       </c>
       <c r="C81" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D81" s="2">
         <v>43979.329918981479</v>
@@ -8363,7 +8373,7 @@
         <v>1.2673174636891871E+18</v>
       </c>
       <c r="C82" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D82" s="2">
         <v>43983.326423611114</v>
@@ -8377,7 +8387,7 @@
         <v>1.267679850996937E+18</v>
       </c>
       <c r="C83" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D83" s="2">
         <v>43984.326423611114</v>
@@ -8391,7 +8401,7 @@
         <v>1.2680434993809039E+18</v>
       </c>
       <c r="C84" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D84" s="2">
         <v>43985.329907407409</v>
@@ -8405,7 +8415,7 @@
         <v>1.2684058861350221E+18</v>
       </c>
       <c r="C85" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D85" s="2">
         <v>43986.329895833333</v>
@@ -8419,7 +8429,7 @@
         <v>1.268768274629759E+18</v>
       </c>
       <c r="C86" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D86" s="2">
         <v>43987.329895833333</v>
@@ -8433,7 +8443,7 @@
         <v>1.26995235389936E+18</v>
       </c>
       <c r="C87" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D87" s="2">
         <v>43990.597337962958</v>
@@ -8447,7 +8457,7 @@
         <v>1.2702116048488161E+18</v>
       </c>
       <c r="C88" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D88" s="2">
         <v>43991.312731481477</v>
@@ -8461,7 +8471,7 @@
         <v>1.2703286074041549E+18</v>
       </c>
       <c r="C89" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D89" s="2">
         <v>43991.635601851849</v>
@@ -8475,7 +8485,7 @@
         <v>1.2705751779282371E+18</v>
       </c>
       <c r="C90" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D90" s="2">
         <v>43992.316006944442</v>
@@ -8489,7 +8499,7 @@
         <v>1.2709401002565839E+18</v>
       </c>
       <c r="C91" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D91" s="2">
         <v>43993.322997685187</v>
@@ -8503,7 +8513,7 @@
         <v>1.2709701653086369E+18</v>
       </c>
       <c r="C92" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D92" s="2">
         <v>43993.405960648153</v>
@@ -8517,7 +8527,7 @@
         <v>1.271004517421781E+18</v>
       </c>
       <c r="C93" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D93" s="2">
         <v>43993.500752314823</v>
@@ -8531,7 +8541,7 @@
         <v>1.2713024845317819E+18</v>
       </c>
       <c r="C94" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D94" s="2">
         <v>43994.32298611111</v>
@@ -8545,7 +8555,7 @@
         <v>1.2717745957297559E+18</v>
       </c>
       <c r="C95" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D95" s="2">
         <v>43995.625763888893</v>
@@ -8559,7 +8569,7 @@
         <v>1.2720613426194839E+18</v>
       </c>
       <c r="C96" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D96" s="2">
         <v>43996.417037037027</v>
@@ -8573,7 +8583,7 @@
         <v>1.2721040051965499E+18</v>
       </c>
       <c r="C97" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D97" s="2">
         <v>43996.534768518519</v>
@@ -8587,7 +8597,7 @@
         <v>1.2723883792048251E+18</v>
       </c>
       <c r="C98" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D98" s="2">
         <v>43997.319490740738</v>
@@ -8601,7 +8611,7 @@
         <v>1.272431292773216E+18</v>
       </c>
       <c r="C99" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D99" s="2">
         <v>43997.437905092593</v>
@@ -8615,7 +8625,7 @@
         <v>1.272752042709332E+18</v>
       </c>
       <c r="C100" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D100" s="2">
         <v>43998.323009259257</v>
@@ -8629,7 +8639,7 @@
         <v>1.2732573667299981E+18</v>
       </c>
       <c r="C101" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D101" s="2">
         <v>43999.717430555553</v>

</xml_diff>